<commit_message>
export lunchList button frontpage and some css-stlye changes on btn
</commit_message>
<xml_diff>
--- a/oppgave_3/files/lunch.xlsx
+++ b/oppgave_3/files/lunch.xlsx
@@ -28,7 +28,7 @@
     <t>Mandag</t>
   </si>
   <si>
-    <t>Trude</t>
+    <t>Simen</t>
   </si>
   <si>
     <t>Fisk</t>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>Torsdag</t>
-  </si>
-  <si>
-    <t>Simen</t>
   </si>
   <si>
     <t>Pizza</t>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>Nora</t>
+  </si>
+  <si>
+    <t>Trude</t>
   </si>
   <si>
     <t>Sharek</t>
@@ -545,10 +545,10 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -556,10 +556,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -573,10 +573,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -587,10 +587,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -601,10 +601,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -615,10 +615,10 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -626,10 +626,10 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -643,7 +643,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
@@ -685,10 +685,10 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -696,10 +696,10 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
         <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -713,7 +713,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
@@ -727,10 +727,10 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -741,10 +741,10 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -755,7 +755,7 @@
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
@@ -766,10 +766,10 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
@@ -783,10 +783,10 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -800,7 +800,7 @@
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -828,7 +828,7 @@
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -836,13 +836,13 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -853,7 +853,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -867,10 +867,10 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -881,7 +881,7 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -895,10 +895,10 @@
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -906,10 +906,10 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
@@ -923,7 +923,7 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
@@ -940,7 +940,7 @@
         <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
         <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -976,10 +976,10 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" t="s">
         <v>9</v>
@@ -996,7 +996,7 @@
         <v>25</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1010,7 +1010,7 @@
         <v>25</v>
       </c>
       <c r="D38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1024,7 +1024,7 @@
         <v>25</v>
       </c>
       <c r="D39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,13 +1046,13 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
         <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1094,7 +1094,7 @@
         <v>24</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1116,13 +1116,13 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C46" t="s">
         <v>27</v>
       </c>
       <c r="D46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1133,10 +1133,10 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1147,7 +1147,7 @@
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
@@ -1161,7 +1161,7 @@
         <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D49" t="s">
         <v>6</v>
@@ -1175,7 +1175,7 @@
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D50" t="s">
         <v>9</v>
@@ -1186,13 +1186,13 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1206,7 +1206,7 @@
         <v>26</v>
       </c>
       <c r="D52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1220,7 +1220,7 @@
         <v>11</v>
       </c>
       <c r="D53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1234,7 +1234,7 @@
         <v>24</v>
       </c>
       <c r="D54" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1256,13 +1256,13 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C56" t="s">
         <v>27</v>
       </c>
       <c r="D56" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1273,10 +1273,10 @@
         <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D57" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1287,7 +1287,7 @@
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D58" t="s">
         <v>9</v>
@@ -1301,10 +1301,10 @@
         <v>10</v>
       </c>
       <c r="C59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1315,10 +1315,10 @@
         <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1326,13 +1326,13 @@
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1360,7 +1360,7 @@
         <v>24</v>
       </c>
       <c r="D63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1371,10 +1371,10 @@
         <v>10</v>
       </c>
       <c r="C64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1388,7 +1388,7 @@
         <v>23</v>
       </c>
       <c r="D65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1396,10 +1396,10 @@
         <v>13</v>
       </c>
       <c r="B66" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" t="s">
         <v>15</v>
-      </c>
-      <c r="C66" t="s">
-        <v>16</v>
       </c>
       <c r="D66" t="s">
         <v>6</v>
@@ -1413,7 +1413,7 @@
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D67" t="s">
         <v>9</v>
@@ -1427,7 +1427,7 @@
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D68" t="s">
         <v>6</v>
@@ -1444,7 +1444,7 @@
         <v>8</v>
       </c>
       <c r="D69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1458,7 +1458,7 @@
         <v>11</v>
       </c>
       <c r="D70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1466,13 +1466,13 @@
         <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C71" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D71" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1486,7 +1486,7 @@
         <v>27</v>
       </c>
       <c r="D72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1511,10 +1511,10 @@
         <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D74" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
         <v>23</v>
       </c>
       <c r="D75" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1536,13 +1536,13 @@
         <v>15</v>
       </c>
       <c r="B76" t="s">
+        <v>14</v>
+      </c>
+      <c r="C76" t="s">
         <v>15</v>
       </c>
-      <c r="C76" t="s">
-        <v>16</v>
-      </c>
       <c r="D76" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1553,10 +1553,10 @@
         <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D77" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1567,10 +1567,10 @@
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D78" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1598,7 +1598,7 @@
         <v>11</v>
       </c>
       <c r="D80" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1606,10 +1606,10 @@
         <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C81" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D81" t="s">
         <v>6</v>
@@ -1637,7 +1637,7 @@
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D83" t="s">
         <v>9</v>
@@ -1651,10 +1651,10 @@
         <v>10</v>
       </c>
       <c r="C84" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D84" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1676,13 +1676,13 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C86" t="s">
         <v>11</v>
       </c>
       <c r="D86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1696,7 +1696,7 @@
         <v>26</v>
       </c>
       <c r="D87" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1707,7 +1707,7 @@
         <v>7</v>
       </c>
       <c r="C88" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D88" t="s">
         <v>6</v>
@@ -1721,7 +1721,7 @@
         <v>10</v>
       </c>
       <c r="C89" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D89" t="s">
         <v>6</v>
@@ -1735,7 +1735,7 @@
         <v>12</v>
       </c>
       <c r="C90" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D90" t="s">
         <v>6</v>
@@ -1746,10 +1746,10 @@
         <v>18</v>
       </c>
       <c r="B91" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C91" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D91" t="s">
         <v>6</v>
@@ -1777,7 +1777,7 @@
         <v>7</v>
       </c>
       <c r="C93" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D93" t="s">
         <v>6</v>
@@ -1791,7 +1791,7 @@
         <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D94" t="s">
         <v>9</v>
@@ -1816,7 +1816,7 @@
         <v>19</v>
       </c>
       <c r="B96" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C96" t="s">
         <v>11</v>
@@ -1836,7 +1836,7 @@
         <v>26</v>
       </c>
       <c r="D97" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1847,10 +1847,10 @@
         <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D98" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1861,7 +1861,7 @@
         <v>10</v>
       </c>
       <c r="C99" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D99" t="s">
         <v>9</v>
@@ -1875,7 +1875,7 @@
         <v>12</v>
       </c>
       <c r="C100" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D100" t="s">
         <v>9</v>
@@ -1886,10 +1886,10 @@
         <v>20</v>
       </c>
       <c r="B101" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C101" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D101" t="s">
         <v>9</v>
@@ -1903,10 +1903,10 @@
         <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D102" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -1920,7 +1920,7 @@
         <v>27</v>
       </c>
       <c r="D103" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -1956,13 +1956,13 @@
         <v>21</v>
       </c>
       <c r="B106" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C106" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D106" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -1973,10 +1973,10 @@
         <v>4</v>
       </c>
       <c r="C107" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D107" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -1987,7 +1987,7 @@
         <v>7</v>
       </c>
       <c r="C108" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D108" t="s">
         <v>6</v>
@@ -2001,7 +2001,7 @@
         <v>10</v>
       </c>
       <c r="C109" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D109" t="s">
         <v>6</v>
@@ -2015,10 +2015,10 @@
         <v>12</v>
       </c>
       <c r="C110" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D110" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2026,10 +2026,10 @@
         <v>22</v>
       </c>
       <c r="B111" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C111" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D111" t="s">
         <v>6</v>
@@ -2043,7 +2043,7 @@
         <v>4</v>
       </c>
       <c r="C112" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D112" t="s">
         <v>6</v>
@@ -2074,7 +2074,7 @@
         <v>8</v>
       </c>
       <c r="D114" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2088,7 +2088,7 @@
         <v>23</v>
       </c>
       <c r="D115" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2096,10 +2096,10 @@
         <v>23</v>
       </c>
       <c r="B116" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C116" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D116" t="s">
         <v>6</v>
@@ -2113,7 +2113,7 @@
         <v>4</v>
       </c>
       <c r="C117" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D117" t="s">
         <v>9</v>
@@ -2127,7 +2127,7 @@
         <v>7</v>
       </c>
       <c r="C118" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D118" t="s">
         <v>9</v>
@@ -2141,7 +2141,7 @@
         <v>10</v>
       </c>
       <c r="C119" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D119" t="s">
         <v>9</v>
@@ -2155,7 +2155,7 @@
         <v>12</v>
       </c>
       <c r="C120" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D120" t="s">
         <v>9</v>
@@ -2166,13 +2166,13 @@
         <v>24</v>
       </c>
       <c r="B121" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C121" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D121" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2183,10 +2183,10 @@
         <v>4</v>
       </c>
       <c r="C122" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D122" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2200,7 +2200,7 @@
         <v>24</v>
       </c>
       <c r="D123" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2214,7 +2214,7 @@
         <v>11</v>
       </c>
       <c r="D124" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2236,13 +2236,13 @@
         <v>25</v>
       </c>
       <c r="B126" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C126" t="s">
         <v>27</v>
       </c>
       <c r="D126" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2267,7 +2267,7 @@
         <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D128" t="s">
         <v>9</v>
@@ -2281,7 +2281,7 @@
         <v>10</v>
       </c>
       <c r="C129" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D129" t="s">
         <v>9</v>
@@ -2295,10 +2295,10 @@
         <v>12</v>
       </c>
       <c r="C130" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D130" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -2306,13 +2306,13 @@
         <v>26</v>
       </c>
       <c r="B131" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C131" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D131" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2323,10 +2323,10 @@
         <v>4</v>
       </c>
       <c r="C132" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D132" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -2354,7 +2354,7 @@
         <v>11</v>
       </c>
       <c r="D134" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -2368,7 +2368,7 @@
         <v>23</v>
       </c>
       <c r="D135" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -2376,7 +2376,7 @@
         <v>27</v>
       </c>
       <c r="B136" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C136" t="s">
         <v>27</v>
@@ -2396,7 +2396,7 @@
         <v>25</v>
       </c>
       <c r="D137" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -2410,7 +2410,7 @@
         <v>25</v>
       </c>
       <c r="D138" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -2446,7 +2446,7 @@
         <v>28</v>
       </c>
       <c r="B141" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C141" t="s">
         <v>25</v>
@@ -2466,7 +2466,7 @@
         <v>25</v>
       </c>
       <c r="D142" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -2508,7 +2508,7 @@
         <v>25</v>
       </c>
       <c r="D145" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -2516,13 +2516,13 @@
         <v>29</v>
       </c>
       <c r="B146" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C146" t="s">
         <v>25</v>
       </c>
       <c r="D146" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -2550,7 +2550,7 @@
         <v>25</v>
       </c>
       <c r="D148" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -2564,7 +2564,7 @@
         <v>25</v>
       </c>
       <c r="D149" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -2578,7 +2578,7 @@
         <v>25</v>
       </c>
       <c r="D150" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -2586,7 +2586,7 @@
         <v>30</v>
       </c>
       <c r="B151" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C151" t="s">
         <v>25</v>
@@ -2606,7 +2606,7 @@
         <v>25</v>
       </c>
       <c r="D152" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -2648,7 +2648,7 @@
         <v>25</v>
       </c>
       <c r="D155" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -2656,7 +2656,7 @@
         <v>31</v>
       </c>
       <c r="B156" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C156" t="s">
         <v>25</v>
@@ -2690,7 +2690,7 @@
         <v>25</v>
       </c>
       <c r="D158" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -2726,13 +2726,13 @@
         <v>32</v>
       </c>
       <c r="B161" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C161" t="s">
         <v>25</v>
       </c>
       <c r="D161" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -2743,7 +2743,7 @@
         <v>4</v>
       </c>
       <c r="C162" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D162" t="s">
         <v>6</v>
@@ -2785,10 +2785,10 @@
         <v>12</v>
       </c>
       <c r="C165" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D165" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -2796,13 +2796,13 @@
         <v>33</v>
       </c>
       <c r="B166" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C166" t="s">
         <v>23</v>
       </c>
       <c r="D166" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -2813,10 +2813,10 @@
         <v>4</v>
       </c>
       <c r="C167" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D167" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -2827,10 +2827,10 @@
         <v>7</v>
       </c>
       <c r="C168" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D168" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -2841,10 +2841,10 @@
         <v>10</v>
       </c>
       <c r="C169" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D169" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -2855,7 +2855,7 @@
         <v>12</v>
       </c>
       <c r="C170" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D170" t="s">
         <v>9</v>
@@ -2866,7 +2866,7 @@
         <v>34</v>
       </c>
       <c r="B171" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C171" t="s">
         <v>8</v>
@@ -2883,10 +2883,10 @@
         <v>4</v>
       </c>
       <c r="C172" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D172" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -2900,7 +2900,7 @@
         <v>24</v>
       </c>
       <c r="D173" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -2925,10 +2925,10 @@
         <v>12</v>
       </c>
       <c r="C175" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D175" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -2936,7 +2936,7 @@
         <v>35</v>
       </c>
       <c r="B176" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C176" t="s">
         <v>23</v>
@@ -2953,7 +2953,7 @@
         <v>4</v>
       </c>
       <c r="C177" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D177" t="s">
         <v>9</v>
@@ -2967,10 +2967,10 @@
         <v>7</v>
       </c>
       <c r="C178" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D178" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -2981,7 +2981,7 @@
         <v>10</v>
       </c>
       <c r="C179" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D179" t="s">
         <v>9</v>
@@ -2995,10 +2995,10 @@
         <v>12</v>
       </c>
       <c r="C180" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D180" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -3006,13 +3006,13 @@
         <v>36</v>
       </c>
       <c r="B181" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C181" t="s">
         <v>8</v>
       </c>
       <c r="D181" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -3026,7 +3026,7 @@
         <v>8</v>
       </c>
       <c r="D182" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -3051,7 +3051,7 @@
         <v>10</v>
       </c>
       <c r="C184" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D184" t="s">
         <v>6</v>
@@ -3065,7 +3065,7 @@
         <v>12</v>
       </c>
       <c r="C185" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D185" t="s">
         <v>9</v>
@@ -3076,7 +3076,7 @@
         <v>37</v>
       </c>
       <c r="B186" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C186" t="s">
         <v>27</v>
@@ -3093,7 +3093,7 @@
         <v>4</v>
       </c>
       <c r="C187" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D187" t="s">
         <v>6</v>
@@ -3107,10 +3107,10 @@
         <v>7</v>
       </c>
       <c r="C188" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D188" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -3124,7 +3124,7 @@
         <v>11</v>
       </c>
       <c r="D189" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -3138,7 +3138,7 @@
         <v>23</v>
       </c>
       <c r="D190" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -3146,10 +3146,10 @@
         <v>38</v>
       </c>
       <c r="B191" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C191" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D191" t="s">
         <v>9</v>
@@ -3166,7 +3166,7 @@
         <v>8</v>
       </c>
       <c r="D192" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -3180,7 +3180,7 @@
         <v>24</v>
       </c>
       <c r="D193" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -3191,7 +3191,7 @@
         <v>10</v>
       </c>
       <c r="C194" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D194" t="s">
         <v>9</v>
@@ -3205,7 +3205,7 @@
         <v>12</v>
       </c>
       <c r="C195" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D195" t="s">
         <v>9</v>
@@ -3216,13 +3216,13 @@
         <v>39</v>
       </c>
       <c r="B196" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C196" t="s">
         <v>27</v>
       </c>
       <c r="D196" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -3250,7 +3250,7 @@
         <v>25</v>
       </c>
       <c r="D198" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -3264,7 +3264,7 @@
         <v>25</v>
       </c>
       <c r="D199" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -3278,7 +3278,7 @@
         <v>25</v>
       </c>
       <c r="D200" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -3286,13 +3286,13 @@
         <v>40</v>
       </c>
       <c r="B201" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C201" t="s">
         <v>25</v>
       </c>
       <c r="D201" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -3306,7 +3306,7 @@
         <v>26</v>
       </c>
       <c r="D202" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -3317,7 +3317,7 @@
         <v>7</v>
       </c>
       <c r="C203" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D203" t="s">
         <v>6</v>
@@ -3334,7 +3334,7 @@
         <v>24</v>
       </c>
       <c r="D204" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -3356,13 +3356,13 @@
         <v>41</v>
       </c>
       <c r="B206" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C206" t="s">
         <v>27</v>
       </c>
       <c r="D206" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -3387,7 +3387,7 @@
         <v>7</v>
       </c>
       <c r="C208" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D208" t="s">
         <v>9</v>
@@ -3415,7 +3415,7 @@
         <v>12</v>
       </c>
       <c r="C210" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D210" t="s">
         <v>9</v>
@@ -3426,10 +3426,10 @@
         <v>42</v>
       </c>
       <c r="B211" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C211" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D211" t="s">
         <v>6</v>
@@ -3457,10 +3457,10 @@
         <v>7</v>
       </c>
       <c r="C213" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D213" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -3474,7 +3474,7 @@
         <v>24</v>
       </c>
       <c r="D214" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -3496,13 +3496,13 @@
         <v>43</v>
       </c>
       <c r="B216" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C216" t="s">
         <v>27</v>
       </c>
       <c r="D216" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -3527,7 +3527,7 @@
         <v>7</v>
       </c>
       <c r="C218" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D218" t="s">
         <v>6</v>
@@ -3555,10 +3555,10 @@
         <v>12</v>
       </c>
       <c r="C220" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D220" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -3566,10 +3566,10 @@
         <v>44</v>
       </c>
       <c r="B221" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C221" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D221" t="s">
         <v>9</v>
@@ -3586,7 +3586,7 @@
         <v>11</v>
       </c>
       <c r="D222" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -3597,7 +3597,7 @@
         <v>7</v>
       </c>
       <c r="C223" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D223" t="s">
         <v>6</v>
@@ -3628,7 +3628,7 @@
         <v>23</v>
       </c>
       <c r="D225" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -3636,13 +3636,13 @@
         <v>45</v>
       </c>
       <c r="B226" t="s">
+        <v>14</v>
+      </c>
+      <c r="C226" t="s">
         <v>15</v>
       </c>
-      <c r="C226" t="s">
-        <v>16</v>
-      </c>
       <c r="D226" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -3653,10 +3653,10 @@
         <v>4</v>
       </c>
       <c r="C227" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D227" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -3667,10 +3667,10 @@
         <v>7</v>
       </c>
       <c r="C228" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D228" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -3681,7 +3681,7 @@
         <v>10</v>
       </c>
       <c r="C229" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D229" t="s">
         <v>9</v>
@@ -3695,7 +3695,7 @@
         <v>12</v>
       </c>
       <c r="C230" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D230" t="s">
         <v>9</v>
@@ -3706,10 +3706,10 @@
         <v>46</v>
       </c>
       <c r="B231" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C231" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D231" t="s">
         <v>6</v>
@@ -3737,10 +3737,10 @@
         <v>7</v>
       </c>
       <c r="C233" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D233" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -3776,13 +3776,13 @@
         <v>47</v>
       </c>
       <c r="B236" t="s">
+        <v>14</v>
+      </c>
+      <c r="C236" t="s">
         <v>15</v>
       </c>
-      <c r="C236" t="s">
-        <v>16</v>
-      </c>
       <c r="D236" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -3793,10 +3793,10 @@
         <v>4</v>
       </c>
       <c r="C237" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D237" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
@@ -3807,10 +3807,10 @@
         <v>7</v>
       </c>
       <c r="C238" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D238" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -3821,10 +3821,10 @@
         <v>10</v>
       </c>
       <c r="C239" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D239" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -3835,10 +3835,10 @@
         <v>12</v>
       </c>
       <c r="C240" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D240" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -3846,10 +3846,10 @@
         <v>48</v>
       </c>
       <c r="B241" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C241" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D241" t="s">
         <v>9</v>
@@ -3866,7 +3866,7 @@
         <v>23</v>
       </c>
       <c r="D242" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -3877,7 +3877,7 @@
         <v>7</v>
       </c>
       <c r="C243" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D243" t="s">
         <v>9</v>
@@ -3894,7 +3894,7 @@
         <v>24</v>
       </c>
       <c r="D244" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -3905,10 +3905,10 @@
         <v>12</v>
       </c>
       <c r="C245" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D245" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -3916,7 +3916,7 @@
         <v>49</v>
       </c>
       <c r="B246" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C246" t="s">
         <v>8</v>
@@ -3947,10 +3947,10 @@
         <v>7</v>
       </c>
       <c r="C248" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D248" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -3961,7 +3961,7 @@
         <v>10</v>
       </c>
       <c r="C249" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D249" t="s">
         <v>6</v>
@@ -3975,10 +3975,10 @@
         <v>12</v>
       </c>
       <c r="C250" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D250" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -3986,13 +3986,13 @@
         <v>50</v>
       </c>
       <c r="B251" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C251" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D251" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -4017,10 +4017,10 @@
         <v>7</v>
       </c>
       <c r="C253" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D253" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
@@ -4045,10 +4045,10 @@
         <v>12</v>
       </c>
       <c r="C255" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D255" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -4056,7 +4056,7 @@
         <v>51</v>
       </c>
       <c r="B256" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C256" t="s">
         <v>8</v>
@@ -4076,7 +4076,7 @@
         <v>25</v>
       </c>
       <c r="D257" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -4090,7 +4090,7 @@
         <v>25</v>
       </c>
       <c r="D258" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -4104,7 +4104,7 @@
         <v>25</v>
       </c>
       <c r="D259" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -4126,7 +4126,7 @@
         <v>52</v>
       </c>
       <c r="B261" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C261" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
seed script changed back
</commit_message>
<xml_diff>
--- a/oppgave_3/files/lunch.xlsx
+++ b/oppgave_3/files/lunch.xlsx
@@ -28,10 +28,10 @@
     <t>Mandag</t>
   </si>
   <si>
-    <t>Simen</t>
+    <t>Trude</t>
   </si>
   <si>
-    <t>Fisk</t>
+    <t>Pasta</t>
   </si>
   <si>
     <t>Tirsdag</t>
@@ -40,7 +40,7 @@
     <t>Sebastian</t>
   </si>
   <si>
-    <t>Taco</t>
+    <t>Pizza</t>
   </si>
   <si>
     <t>Onsdag</t>
@@ -49,10 +49,16 @@
     <t>Lars</t>
   </si>
   <si>
+    <t>Taco</t>
+  </si>
+  <si>
     <t>Torsdag</t>
   </si>
   <si>
-    <t>Pizza</t>
+    <t>Simen</t>
+  </si>
+  <si>
+    <t>Fisk</t>
   </si>
   <si>
     <t>Fredag</t>
@@ -62,9 +68,6 @@
   </si>
   <si>
     <t>Olav</t>
-  </si>
-  <si>
-    <t>Pasta</t>
   </si>
   <si>
     <t>Trine</t>
@@ -77,9 +80,6 @@
   </si>
   <si>
     <t>Nora</t>
-  </si>
-  <si>
-    <t>Trude</t>
   </si>
   <si>
     <t>Sharek</t>
@@ -534,7 +534,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -542,13 +542,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -556,13 +556,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -573,10 +573,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -587,10 +587,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -601,10 +601,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -612,13 +612,13 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -626,13 +626,13 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -643,10 +643,10 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -674,7 +674,7 @@
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -682,13 +682,13 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -696,13 +696,13 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -713,10 +713,10 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -727,10 +727,10 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -741,10 +741,10 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -752,10 +752,10 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
@@ -766,13 +766,13 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -783,10 +783,10 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -800,7 +800,7 @@
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -814,7 +814,7 @@
         <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -822,13 +822,13 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -836,13 +836,13 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -853,10 +853,10 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -867,10 +867,10 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -881,10 +881,10 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -892,13 +892,13 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -906,13 +906,13 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -923,10 +923,10 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -940,7 +940,7 @@
         <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
         <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -962,13 +962,13 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -976,13 +976,13 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -996,7 +996,7 @@
         <v>25</v>
       </c>
       <c r="D37" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1010,7 +1010,7 @@
         <v>25</v>
       </c>
       <c r="D38" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1024,7 +1024,7 @@
         <v>25</v>
       </c>
       <c r="D39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1032,13 +1032,13 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
         <v>25</v>
       </c>
       <c r="D40" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,13 +1046,13 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C41" t="s">
         <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1094,7 +1094,7 @@
         <v>24</v>
       </c>
       <c r="D44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1102,13 +1102,13 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C45" t="s">
         <v>23</v>
       </c>
       <c r="D45" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1116,13 +1116,13 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C46" t="s">
         <v>27</v>
       </c>
       <c r="D46" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1133,10 +1133,10 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1147,10 +1147,10 @@
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D48" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1161,10 +1161,10 @@
         <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1172,13 +1172,13 @@
         <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1186,13 +1186,13 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C51" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1206,7 +1206,7 @@
         <v>26</v>
       </c>
       <c r="D52" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1220,7 +1220,7 @@
         <v>11</v>
       </c>
       <c r="D53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1234,7 +1234,7 @@
         <v>24</v>
       </c>
       <c r="D54" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1242,7 +1242,7 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C55" t="s">
         <v>23</v>
@@ -1256,13 +1256,13 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C56" t="s">
         <v>27</v>
       </c>
       <c r="D56" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1273,10 +1273,10 @@
         <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D57" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1287,10 +1287,10 @@
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D58" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1301,10 +1301,10 @@
         <v>10</v>
       </c>
       <c r="C59" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D59" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1312,13 +1312,13 @@
         <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D60" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1326,13 +1326,13 @@
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C61" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1346,7 +1346,7 @@
         <v>27</v>
       </c>
       <c r="D62" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1360,7 +1360,7 @@
         <v>24</v>
       </c>
       <c r="D63" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1371,10 +1371,10 @@
         <v>10</v>
       </c>
       <c r="C64" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D64" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1382,13 +1382,13 @@
         <v>13</v>
       </c>
       <c r="B65" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C65" t="s">
         <v>23</v>
       </c>
       <c r="D65" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1396,10 +1396,10 @@
         <v>13</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C66" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D66" t="s">
         <v>6</v>
@@ -1413,10 +1413,10 @@
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D67" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1427,10 +1427,10 @@
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D68" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1444,7 +1444,7 @@
         <v>8</v>
       </c>
       <c r="D69" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1452,13 +1452,13 @@
         <v>14</v>
       </c>
       <c r="B70" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C70" t="s">
         <v>11</v>
       </c>
       <c r="D70" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1466,13 +1466,13 @@
         <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C71" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D71" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1486,7 +1486,7 @@
         <v>27</v>
       </c>
       <c r="D72" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1511,10 +1511,10 @@
         <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D74" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1522,13 +1522,13 @@
         <v>15</v>
       </c>
       <c r="B75" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C75" t="s">
         <v>23</v>
       </c>
       <c r="D75" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1536,13 +1536,13 @@
         <v>15</v>
       </c>
       <c r="B76" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C76" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D76" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1553,10 +1553,10 @@
         <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D77" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1567,10 +1567,10 @@
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D78" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1584,7 +1584,7 @@
         <v>8</v>
       </c>
       <c r="D79" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1592,13 +1592,13 @@
         <v>16</v>
       </c>
       <c r="B80" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C80" t="s">
         <v>11</v>
       </c>
       <c r="D80" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1606,13 +1606,13 @@
         <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C81" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D81" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1637,7 +1637,7 @@
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D83" t="s">
         <v>9</v>
@@ -1651,10 +1651,10 @@
         <v>10</v>
       </c>
       <c r="C84" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D84" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1662,7 +1662,7 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
@@ -1676,13 +1676,13 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C86" t="s">
         <v>11</v>
       </c>
       <c r="D86" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1696,7 +1696,7 @@
         <v>26</v>
       </c>
       <c r="D87" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1707,10 +1707,10 @@
         <v>7</v>
       </c>
       <c r="C88" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D88" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1721,10 +1721,10 @@
         <v>10</v>
       </c>
       <c r="C89" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D89" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1732,13 +1732,13 @@
         <v>18</v>
       </c>
       <c r="B90" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C90" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D90" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -1746,10 +1746,10 @@
         <v>18</v>
       </c>
       <c r="B91" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C91" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D91" t="s">
         <v>6</v>
@@ -1766,7 +1766,7 @@
         <v>27</v>
       </c>
       <c r="D92" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1777,7 +1777,7 @@
         <v>7</v>
       </c>
       <c r="C93" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D93" t="s">
         <v>6</v>
@@ -1791,10 +1791,10 @@
         <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D94" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -1802,7 +1802,7 @@
         <v>19</v>
       </c>
       <c r="B95" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C95" t="s">
         <v>8</v>
@@ -1816,13 +1816,13 @@
         <v>19</v>
       </c>
       <c r="B96" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C96" t="s">
         <v>11</v>
       </c>
       <c r="D96" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -1836,7 +1836,7 @@
         <v>26</v>
       </c>
       <c r="D97" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1847,10 +1847,10 @@
         <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D98" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1861,7 +1861,7 @@
         <v>10</v>
       </c>
       <c r="C99" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D99" t="s">
         <v>9</v>
@@ -1872,13 +1872,13 @@
         <v>20</v>
       </c>
       <c r="B100" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C100" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D100" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -1886,13 +1886,13 @@
         <v>20</v>
       </c>
       <c r="B101" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C101" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D101" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -1903,10 +1903,10 @@
         <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D102" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -1920,7 +1920,7 @@
         <v>27</v>
       </c>
       <c r="D103" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -1934,7 +1934,7 @@
         <v>8</v>
       </c>
       <c r="D104" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -1942,13 +1942,13 @@
         <v>21</v>
       </c>
       <c r="B105" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C105" t="s">
         <v>23</v>
       </c>
       <c r="D105" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -1956,13 +1956,13 @@
         <v>21</v>
       </c>
       <c r="B106" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C106" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D106" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -1973,10 +1973,10 @@
         <v>4</v>
       </c>
       <c r="C107" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D107" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -1987,10 +1987,10 @@
         <v>7</v>
       </c>
       <c r="C108" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D108" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2001,10 +2001,10 @@
         <v>10</v>
       </c>
       <c r="C109" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D109" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2012,13 +2012,13 @@
         <v>22</v>
       </c>
       <c r="B110" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C110" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D110" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2026,13 +2026,13 @@
         <v>22</v>
       </c>
       <c r="B111" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C111" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D111" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2043,10 +2043,10 @@
         <v>4</v>
       </c>
       <c r="C112" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D112" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2060,7 +2060,7 @@
         <v>27</v>
       </c>
       <c r="D113" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2074,7 +2074,7 @@
         <v>8</v>
       </c>
       <c r="D114" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2082,13 +2082,13 @@
         <v>23</v>
       </c>
       <c r="B115" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C115" t="s">
         <v>23</v>
       </c>
       <c r="D115" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2096,13 +2096,13 @@
         <v>23</v>
       </c>
       <c r="B116" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C116" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D116" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2113,10 +2113,10 @@
         <v>4</v>
       </c>
       <c r="C117" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D117" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2127,7 +2127,7 @@
         <v>7</v>
       </c>
       <c r="C118" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D118" t="s">
         <v>9</v>
@@ -2141,10 +2141,10 @@
         <v>10</v>
       </c>
       <c r="C119" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D119" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2152,13 +2152,13 @@
         <v>24</v>
       </c>
       <c r="B120" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C120" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D120" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2166,13 +2166,13 @@
         <v>24</v>
       </c>
       <c r="B121" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C121" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D121" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2183,10 +2183,10 @@
         <v>4</v>
       </c>
       <c r="C122" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D122" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2200,7 +2200,7 @@
         <v>24</v>
       </c>
       <c r="D123" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2214,7 +2214,7 @@
         <v>11</v>
       </c>
       <c r="D124" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2222,7 +2222,7 @@
         <v>25</v>
       </c>
       <c r="B125" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C125" t="s">
         <v>23</v>
@@ -2236,13 +2236,13 @@
         <v>25</v>
       </c>
       <c r="B126" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C126" t="s">
         <v>27</v>
       </c>
       <c r="D126" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2256,7 +2256,7 @@
         <v>8</v>
       </c>
       <c r="D127" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -2267,10 +2267,10 @@
         <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D128" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -2281,10 +2281,10 @@
         <v>10</v>
       </c>
       <c r="C129" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D129" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -2292,13 +2292,13 @@
         <v>26</v>
       </c>
       <c r="B130" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C130" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D130" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -2306,13 +2306,13 @@
         <v>26</v>
       </c>
       <c r="B131" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C131" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D131" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2323,10 +2323,10 @@
         <v>4</v>
       </c>
       <c r="C132" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D132" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -2354,7 +2354,7 @@
         <v>11</v>
       </c>
       <c r="D134" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -2362,13 +2362,13 @@
         <v>27</v>
       </c>
       <c r="B135" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C135" t="s">
         <v>23</v>
       </c>
       <c r="D135" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -2376,13 +2376,13 @@
         <v>27</v>
       </c>
       <c r="B136" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C136" t="s">
         <v>27</v>
       </c>
       <c r="D136" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -2396,7 +2396,7 @@
         <v>25</v>
       </c>
       <c r="D137" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -2410,7 +2410,7 @@
         <v>25</v>
       </c>
       <c r="D138" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -2424,7 +2424,7 @@
         <v>25</v>
       </c>
       <c r="D139" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -2432,7 +2432,7 @@
         <v>28</v>
       </c>
       <c r="B140" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C140" t="s">
         <v>25</v>
@@ -2446,13 +2446,13 @@
         <v>28</v>
       </c>
       <c r="B141" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C141" t="s">
         <v>25</v>
       </c>
       <c r="D141" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -2466,7 +2466,7 @@
         <v>25</v>
       </c>
       <c r="D142" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -2480,7 +2480,7 @@
         <v>25</v>
       </c>
       <c r="D143" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -2494,7 +2494,7 @@
         <v>25</v>
       </c>
       <c r="D144" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -2502,13 +2502,13 @@
         <v>29</v>
       </c>
       <c r="B145" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C145" t="s">
         <v>25</v>
       </c>
       <c r="D145" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -2516,13 +2516,13 @@
         <v>29</v>
       </c>
       <c r="B146" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C146" t="s">
         <v>25</v>
       </c>
       <c r="D146" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -2550,7 +2550,7 @@
         <v>25</v>
       </c>
       <c r="D148" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -2564,7 +2564,7 @@
         <v>25</v>
       </c>
       <c r="D149" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -2572,13 +2572,13 @@
         <v>30</v>
       </c>
       <c r="B150" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C150" t="s">
         <v>25</v>
       </c>
       <c r="D150" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -2586,13 +2586,13 @@
         <v>30</v>
       </c>
       <c r="B151" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C151" t="s">
         <v>25</v>
       </c>
       <c r="D151" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -2606,7 +2606,7 @@
         <v>25</v>
       </c>
       <c r="D152" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -2620,7 +2620,7 @@
         <v>25</v>
       </c>
       <c r="D153" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -2642,13 +2642,13 @@
         <v>31</v>
       </c>
       <c r="B155" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C155" t="s">
         <v>25</v>
       </c>
       <c r="D155" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -2656,13 +2656,13 @@
         <v>31</v>
       </c>
       <c r="B156" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C156" t="s">
         <v>25</v>
       </c>
       <c r="D156" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -2690,7 +2690,7 @@
         <v>25</v>
       </c>
       <c r="D158" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -2704,7 +2704,7 @@
         <v>25</v>
       </c>
       <c r="D159" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -2712,13 +2712,13 @@
         <v>32</v>
       </c>
       <c r="B160" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C160" t="s">
         <v>25</v>
       </c>
       <c r="D160" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -2726,13 +2726,13 @@
         <v>32</v>
       </c>
       <c r="B161" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C161" t="s">
         <v>25</v>
       </c>
       <c r="D161" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -2743,7 +2743,7 @@
         <v>4</v>
       </c>
       <c r="C162" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D162" t="s">
         <v>6</v>
@@ -2760,7 +2760,7 @@
         <v>24</v>
       </c>
       <c r="D163" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -2774,7 +2774,7 @@
         <v>27</v>
       </c>
       <c r="D164" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -2782,13 +2782,13 @@
         <v>33</v>
       </c>
       <c r="B165" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C165" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D165" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -2796,13 +2796,13 @@
         <v>33</v>
       </c>
       <c r="B166" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C166" t="s">
         <v>23</v>
       </c>
       <c r="D166" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -2813,10 +2813,10 @@
         <v>4</v>
       </c>
       <c r="C167" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D167" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -2827,10 +2827,10 @@
         <v>7</v>
       </c>
       <c r="C168" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D168" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -2841,10 +2841,10 @@
         <v>10</v>
       </c>
       <c r="C169" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D169" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -2852,13 +2852,13 @@
         <v>34</v>
       </c>
       <c r="B170" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C170" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D170" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -2866,13 +2866,13 @@
         <v>34</v>
       </c>
       <c r="B171" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C171" t="s">
         <v>8</v>
       </c>
       <c r="D171" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -2883,10 +2883,10 @@
         <v>4</v>
       </c>
       <c r="C172" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D172" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -2900,7 +2900,7 @@
         <v>24</v>
       </c>
       <c r="D173" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -2914,7 +2914,7 @@
         <v>27</v>
       </c>
       <c r="D174" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -2922,13 +2922,13 @@
         <v>35</v>
       </c>
       <c r="B175" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C175" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D175" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -2936,13 +2936,13 @@
         <v>35</v>
       </c>
       <c r="B176" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C176" t="s">
         <v>23</v>
       </c>
       <c r="D176" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -2953,10 +2953,10 @@
         <v>4</v>
       </c>
       <c r="C177" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D177" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -2967,10 +2967,10 @@
         <v>7</v>
       </c>
       <c r="C178" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D178" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -2981,10 +2981,10 @@
         <v>10</v>
       </c>
       <c r="C179" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D179" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -2992,13 +2992,13 @@
         <v>36</v>
       </c>
       <c r="B180" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C180" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D180" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -3006,13 +3006,13 @@
         <v>36</v>
       </c>
       <c r="B181" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C181" t="s">
         <v>8</v>
       </c>
       <c r="D181" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -3026,7 +3026,7 @@
         <v>8</v>
       </c>
       <c r="D182" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -3040,7 +3040,7 @@
         <v>24</v>
       </c>
       <c r="D183" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -3051,10 +3051,10 @@
         <v>10</v>
       </c>
       <c r="C184" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D184" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -3062,13 +3062,13 @@
         <v>37</v>
       </c>
       <c r="B185" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C185" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D185" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -3076,13 +3076,13 @@
         <v>37</v>
       </c>
       <c r="B186" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C186" t="s">
         <v>27</v>
       </c>
       <c r="D186" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -3093,10 +3093,10 @@
         <v>4</v>
       </c>
       <c r="C187" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D187" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -3107,10 +3107,10 @@
         <v>7</v>
       </c>
       <c r="C188" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D188" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -3124,7 +3124,7 @@
         <v>11</v>
       </c>
       <c r="D189" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -3132,13 +3132,13 @@
         <v>38</v>
       </c>
       <c r="B190" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C190" t="s">
         <v>23</v>
       </c>
       <c r="D190" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -3146,10 +3146,10 @@
         <v>38</v>
       </c>
       <c r="B191" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C191" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D191" t="s">
         <v>9</v>
@@ -3166,7 +3166,7 @@
         <v>8</v>
       </c>
       <c r="D192" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -3180,7 +3180,7 @@
         <v>24</v>
       </c>
       <c r="D193" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -3191,10 +3191,10 @@
         <v>10</v>
       </c>
       <c r="C194" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D194" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -3202,10 +3202,10 @@
         <v>39</v>
       </c>
       <c r="B195" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C195" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D195" t="s">
         <v>9</v>
@@ -3216,13 +3216,13 @@
         <v>39</v>
       </c>
       <c r="B196" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C196" t="s">
         <v>27</v>
       </c>
       <c r="D196" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -3236,7 +3236,7 @@
         <v>25</v>
       </c>
       <c r="D197" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -3250,7 +3250,7 @@
         <v>25</v>
       </c>
       <c r="D198" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -3264,7 +3264,7 @@
         <v>25</v>
       </c>
       <c r="D199" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -3272,13 +3272,13 @@
         <v>40</v>
       </c>
       <c r="B200" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C200" t="s">
         <v>25</v>
       </c>
       <c r="D200" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -3286,13 +3286,13 @@
         <v>40</v>
       </c>
       <c r="B201" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C201" t="s">
         <v>25</v>
       </c>
       <c r="D201" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -3306,7 +3306,7 @@
         <v>26</v>
       </c>
       <c r="D202" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -3317,10 +3317,10 @@
         <v>7</v>
       </c>
       <c r="C203" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D203" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -3334,7 +3334,7 @@
         <v>24</v>
       </c>
       <c r="D204" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -3342,7 +3342,7 @@
         <v>41</v>
       </c>
       <c r="B205" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C205" t="s">
         <v>11</v>
@@ -3356,13 +3356,13 @@
         <v>41</v>
       </c>
       <c r="B206" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C206" t="s">
         <v>27</v>
       </c>
       <c r="D206" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -3387,10 +3387,10 @@
         <v>7</v>
       </c>
       <c r="C208" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D208" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -3404,7 +3404,7 @@
         <v>23</v>
       </c>
       <c r="D209" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -3412,13 +3412,13 @@
         <v>42</v>
       </c>
       <c r="B210" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C210" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D210" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -3426,13 +3426,13 @@
         <v>42</v>
       </c>
       <c r="B211" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C211" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D211" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -3446,7 +3446,7 @@
         <v>26</v>
       </c>
       <c r="D212" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -3457,10 +3457,10 @@
         <v>7</v>
       </c>
       <c r="C213" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D213" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -3474,7 +3474,7 @@
         <v>24</v>
       </c>
       <c r="D214" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -3482,7 +3482,7 @@
         <v>43</v>
       </c>
       <c r="B215" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C215" t="s">
         <v>11</v>
@@ -3496,13 +3496,13 @@
         <v>43</v>
       </c>
       <c r="B216" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C216" t="s">
         <v>27</v>
       </c>
       <c r="D216" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -3516,7 +3516,7 @@
         <v>8</v>
       </c>
       <c r="D217" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -3527,10 +3527,10 @@
         <v>7</v>
       </c>
       <c r="C218" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D218" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -3552,13 +3552,13 @@
         <v>44</v>
       </c>
       <c r="B220" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C220" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D220" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -3566,13 +3566,13 @@
         <v>44</v>
       </c>
       <c r="B221" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C221" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D221" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -3586,7 +3586,7 @@
         <v>11</v>
       </c>
       <c r="D222" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -3597,7 +3597,7 @@
         <v>7</v>
       </c>
       <c r="C223" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D223" t="s">
         <v>6</v>
@@ -3614,7 +3614,7 @@
         <v>24</v>
       </c>
       <c r="D224" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -3622,13 +3622,13 @@
         <v>45</v>
       </c>
       <c r="B225" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C225" t="s">
         <v>23</v>
       </c>
       <c r="D225" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -3636,13 +3636,13 @@
         <v>45</v>
       </c>
       <c r="B226" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C226" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D226" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -3653,10 +3653,10 @@
         <v>4</v>
       </c>
       <c r="C227" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D227" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -3667,10 +3667,10 @@
         <v>7</v>
       </c>
       <c r="C228" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D228" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -3681,7 +3681,7 @@
         <v>10</v>
       </c>
       <c r="C229" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D229" t="s">
         <v>9</v>
@@ -3692,10 +3692,10 @@
         <v>46</v>
       </c>
       <c r="B230" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C230" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D230" t="s">
         <v>9</v>
@@ -3706,13 +3706,13 @@
         <v>46</v>
       </c>
       <c r="B231" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C231" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D231" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -3726,7 +3726,7 @@
         <v>11</v>
       </c>
       <c r="D232" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -3737,10 +3737,10 @@
         <v>7</v>
       </c>
       <c r="C233" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D233" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -3754,7 +3754,7 @@
         <v>24</v>
       </c>
       <c r="D234" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -3762,13 +3762,13 @@
         <v>47</v>
       </c>
       <c r="B235" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C235" t="s">
         <v>23</v>
       </c>
       <c r="D235" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -3776,13 +3776,13 @@
         <v>47</v>
       </c>
       <c r="B236" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C236" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D236" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -3793,10 +3793,10 @@
         <v>4</v>
       </c>
       <c r="C237" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D237" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
@@ -3807,10 +3807,10 @@
         <v>7</v>
       </c>
       <c r="C238" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D238" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -3821,10 +3821,10 @@
         <v>10</v>
       </c>
       <c r="C239" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D239" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -3832,13 +3832,13 @@
         <v>48</v>
       </c>
       <c r="B240" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C240" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D240" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -3846,13 +3846,13 @@
         <v>48</v>
       </c>
       <c r="B241" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C241" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D241" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -3866,7 +3866,7 @@
         <v>23</v>
       </c>
       <c r="D242" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -3877,10 +3877,10 @@
         <v>7</v>
       </c>
       <c r="C243" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D243" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -3894,7 +3894,7 @@
         <v>24</v>
       </c>
       <c r="D244" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -3902,13 +3902,13 @@
         <v>49</v>
       </c>
       <c r="B245" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C245" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D245" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -3916,7 +3916,7 @@
         <v>49</v>
       </c>
       <c r="B246" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C246" t="s">
         <v>8</v>
@@ -3936,7 +3936,7 @@
         <v>11</v>
       </c>
       <c r="D247" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -3947,10 +3947,10 @@
         <v>7</v>
       </c>
       <c r="C248" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D248" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -3961,10 +3961,10 @@
         <v>10</v>
       </c>
       <c r="C249" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D249" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -3972,13 +3972,13 @@
         <v>50</v>
       </c>
       <c r="B250" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C250" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D250" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -3986,13 +3986,13 @@
         <v>50</v>
       </c>
       <c r="B251" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C251" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D251" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -4006,7 +4006,7 @@
         <v>23</v>
       </c>
       <c r="D252" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
@@ -4017,10 +4017,10 @@
         <v>7</v>
       </c>
       <c r="C253" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D253" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
@@ -4034,7 +4034,7 @@
         <v>24</v>
       </c>
       <c r="D254" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -4042,13 +4042,13 @@
         <v>51</v>
       </c>
       <c r="B255" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C255" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D255" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -4056,13 +4056,13 @@
         <v>51</v>
       </c>
       <c r="B256" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C256" t="s">
         <v>8</v>
       </c>
       <c r="D256" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -4076,7 +4076,7 @@
         <v>25</v>
       </c>
       <c r="D257" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -4090,7 +4090,7 @@
         <v>25</v>
       </c>
       <c r="D258" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -4104,7 +4104,7 @@
         <v>25</v>
       </c>
       <c r="D259" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -4112,13 +4112,13 @@
         <v>52</v>
       </c>
       <c r="B260" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C260" t="s">
         <v>25</v>
       </c>
       <c r="D260" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -4126,13 +4126,13 @@
         <v>52</v>
       </c>
       <c r="B261" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C261" t="s">
         <v>25</v>
       </c>
       <c r="D261" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
overrideEmploeeForm is now fetching employee list from api
</commit_message>
<xml_diff>
--- a/oppgave_3/files/lunch.xlsx
+++ b/oppgave_3/files/lunch.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="29">
   <si>
     <t>Week Number</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Mandag</t>
   </si>
   <si>
-    <t>Trude</t>
+    <t>Philip</t>
   </si>
   <si>
     <t>Pasta</t>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Nora</t>
+  </si>
+  <si>
+    <t>Trude</t>
   </si>
   <si>
     <t>Sharek</t>
@@ -643,7 +646,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -797,7 +800,7 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -811,7 +814,7 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -853,7 +856,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
@@ -937,7 +940,7 @@
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
@@ -951,7 +954,7 @@
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
         <v>15</v>
@@ -993,7 +996,7 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D37" t="s">
         <v>9</v>
@@ -1007,7 +1010,7 @@
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
@@ -1021,7 +1024,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D39" t="s">
         <v>15</v>
@@ -1035,7 +1038,7 @@
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -1049,7 +1052,7 @@
         <v>16</v>
       </c>
       <c r="C41" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D41" t="s">
         <v>15</v>
@@ -1063,7 +1066,7 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
@@ -1091,7 +1094,7 @@
         <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -1105,7 +1108,7 @@
         <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
@@ -1119,7 +1122,7 @@
         <v>16</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -1133,7 +1136,7 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
@@ -1203,7 +1206,7 @@
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
@@ -1231,7 +1234,7 @@
         <v>10</v>
       </c>
       <c r="C54" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D54" t="s">
         <v>6</v>
@@ -1245,7 +1248,7 @@
         <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D55" t="s">
         <v>6</v>
@@ -1259,7 +1262,7 @@
         <v>16</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D56" t="s">
         <v>15</v>
@@ -1273,7 +1276,7 @@
         <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D57" t="s">
         <v>9</v>
@@ -1343,7 +1346,7 @@
         <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D62" t="s">
         <v>12</v>
@@ -1357,7 +1360,7 @@
         <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
@@ -1385,7 +1388,7 @@
         <v>13</v>
       </c>
       <c r="C65" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D65" t="s">
         <v>6</v>
@@ -1483,7 +1486,7 @@
         <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D72" t="s">
         <v>15</v>
@@ -1497,7 +1500,7 @@
         <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D73" t="s">
         <v>9</v>
@@ -1525,7 +1528,7 @@
         <v>13</v>
       </c>
       <c r="C75" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D75" t="s">
         <v>15</v>
@@ -1623,7 +1626,7 @@
         <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D82" t="s">
         <v>9</v>
@@ -1693,7 +1696,7 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D87" t="s">
         <v>6</v>
@@ -1707,7 +1710,7 @@
         <v>7</v>
       </c>
       <c r="C88" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D88" t="s">
         <v>12</v>
@@ -1763,7 +1766,7 @@
         <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D92" t="s">
         <v>12</v>
@@ -1833,7 +1836,7 @@
         <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D97" t="s">
         <v>6</v>
@@ -1847,7 +1850,7 @@
         <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D98" t="s">
         <v>6</v>
@@ -1917,7 +1920,7 @@
         <v>7</v>
       </c>
       <c r="C103" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D103" t="s">
         <v>12</v>
@@ -1945,7 +1948,7 @@
         <v>13</v>
       </c>
       <c r="C105" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D105" t="s">
         <v>15</v>
@@ -1973,7 +1976,7 @@
         <v>4</v>
       </c>
       <c r="C107" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D107" t="s">
         <v>12</v>
@@ -2057,7 +2060,7 @@
         <v>7</v>
       </c>
       <c r="C113" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D113" t="s">
         <v>12</v>
@@ -2085,7 +2088,7 @@
         <v>13</v>
       </c>
       <c r="C115" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D115" t="s">
         <v>9</v>
@@ -2113,7 +2116,7 @@
         <v>4</v>
       </c>
       <c r="C117" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D117" t="s">
         <v>12</v>
@@ -2197,7 +2200,7 @@
         <v>7</v>
       </c>
       <c r="C123" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D123" t="s">
         <v>9</v>
@@ -2225,7 +2228,7 @@
         <v>13</v>
       </c>
       <c r="C125" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D125" t="s">
         <v>9</v>
@@ -2239,7 +2242,7 @@
         <v>16</v>
       </c>
       <c r="C126" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D126" t="s">
         <v>15</v>
@@ -2267,7 +2270,7 @@
         <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D128" t="s">
         <v>15</v>
@@ -2337,7 +2340,7 @@
         <v>7</v>
       </c>
       <c r="C133" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D133" t="s">
         <v>9</v>
@@ -2365,7 +2368,7 @@
         <v>13</v>
       </c>
       <c r="C135" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D135" t="s">
         <v>6</v>
@@ -2379,7 +2382,7 @@
         <v>16</v>
       </c>
       <c r="C136" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D136" t="s">
         <v>15</v>
@@ -2393,7 +2396,7 @@
         <v>4</v>
       </c>
       <c r="C137" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D137" t="s">
         <v>9</v>
@@ -2407,7 +2410,7 @@
         <v>7</v>
       </c>
       <c r="C138" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D138" t="s">
         <v>6</v>
@@ -2421,7 +2424,7 @@
         <v>10</v>
       </c>
       <c r="C139" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D139" t="s">
         <v>15</v>
@@ -2435,7 +2438,7 @@
         <v>13</v>
       </c>
       <c r="C140" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D140" t="s">
         <v>9</v>
@@ -2449,7 +2452,7 @@
         <v>16</v>
       </c>
       <c r="C141" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D141" t="s">
         <v>15</v>
@@ -2463,7 +2466,7 @@
         <v>4</v>
       </c>
       <c r="C142" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D142" t="s">
         <v>6</v>
@@ -2477,7 +2480,7 @@
         <v>7</v>
       </c>
       <c r="C143" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D143" t="s">
         <v>15</v>
@@ -2491,7 +2494,7 @@
         <v>10</v>
       </c>
       <c r="C144" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D144" t="s">
         <v>15</v>
@@ -2505,7 +2508,7 @@
         <v>13</v>
       </c>
       <c r="C145" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D145" t="s">
         <v>12</v>
@@ -2519,7 +2522,7 @@
         <v>16</v>
       </c>
       <c r="C146" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D146" t="s">
         <v>12</v>
@@ -2533,7 +2536,7 @@
         <v>4</v>
       </c>
       <c r="C147" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D147" t="s">
         <v>6</v>
@@ -2547,7 +2550,7 @@
         <v>7</v>
       </c>
       <c r="C148" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D148" t="s">
         <v>9</v>
@@ -2561,7 +2564,7 @@
         <v>10</v>
       </c>
       <c r="C149" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D149" t="s">
         <v>15</v>
@@ -2575,7 +2578,7 @@
         <v>13</v>
       </c>
       <c r="C150" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D150" t="s">
         <v>15</v>
@@ -2589,7 +2592,7 @@
         <v>16</v>
       </c>
       <c r="C151" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D151" t="s">
         <v>15</v>
@@ -2603,7 +2606,7 @@
         <v>4</v>
       </c>
       <c r="C152" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D152" t="s">
         <v>12</v>
@@ -2617,7 +2620,7 @@
         <v>7</v>
       </c>
       <c r="C153" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D153" t="s">
         <v>12</v>
@@ -2631,7 +2634,7 @@
         <v>10</v>
       </c>
       <c r="C154" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D154" t="s">
         <v>6</v>
@@ -2645,7 +2648,7 @@
         <v>13</v>
       </c>
       <c r="C155" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D155" t="s">
         <v>6</v>
@@ -2659,7 +2662,7 @@
         <v>16</v>
       </c>
       <c r="C156" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D156" t="s">
         <v>9</v>
@@ -2673,7 +2676,7 @@
         <v>4</v>
       </c>
       <c r="C157" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D157" t="s">
         <v>9</v>
@@ -2687,7 +2690,7 @@
         <v>7</v>
       </c>
       <c r="C158" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D158" t="s">
         <v>9</v>
@@ -2701,7 +2704,7 @@
         <v>10</v>
       </c>
       <c r="C159" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D159" t="s">
         <v>12</v>
@@ -2715,7 +2718,7 @@
         <v>13</v>
       </c>
       <c r="C160" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D160" t="s">
         <v>6</v>
@@ -2729,7 +2732,7 @@
         <v>16</v>
       </c>
       <c r="C161" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D161" t="s">
         <v>12</v>
@@ -2757,7 +2760,7 @@
         <v>7</v>
       </c>
       <c r="C163" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D163" t="s">
         <v>15</v>
@@ -2771,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="C164" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D164" t="s">
         <v>15</v>
@@ -2799,7 +2802,7 @@
         <v>16</v>
       </c>
       <c r="C166" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D166" t="s">
         <v>9</v>
@@ -2827,7 +2830,7 @@
         <v>7</v>
       </c>
       <c r="C168" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D168" t="s">
         <v>9</v>
@@ -2897,7 +2900,7 @@
         <v>7</v>
       </c>
       <c r="C173" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D173" t="s">
         <v>15</v>
@@ -2911,7 +2914,7 @@
         <v>10</v>
       </c>
       <c r="C174" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D174" t="s">
         <v>15</v>
@@ -2939,7 +2942,7 @@
         <v>16</v>
       </c>
       <c r="C176" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D176" t="s">
         <v>15</v>
@@ -2967,7 +2970,7 @@
         <v>7</v>
       </c>
       <c r="C178" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D178" t="s">
         <v>9</v>
@@ -3037,7 +3040,7 @@
         <v>7</v>
       </c>
       <c r="C183" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D183" t="s">
         <v>12</v>
@@ -3079,7 +3082,7 @@
         <v>16</v>
       </c>
       <c r="C186" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D186" t="s">
         <v>12</v>
@@ -3093,7 +3096,7 @@
         <v>4</v>
       </c>
       <c r="C187" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D187" t="s">
         <v>9</v>
@@ -3135,7 +3138,7 @@
         <v>13</v>
       </c>
       <c r="C190" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D190" t="s">
         <v>12</v>
@@ -3177,7 +3180,7 @@
         <v>7</v>
       </c>
       <c r="C193" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D193" t="s">
         <v>12</v>
@@ -3219,7 +3222,7 @@
         <v>16</v>
       </c>
       <c r="C196" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D196" t="s">
         <v>15</v>
@@ -3233,7 +3236,7 @@
         <v>4</v>
       </c>
       <c r="C197" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D197" t="s">
         <v>15</v>
@@ -3247,7 +3250,7 @@
         <v>7</v>
       </c>
       <c r="C198" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D198" t="s">
         <v>6</v>
@@ -3261,7 +3264,7 @@
         <v>10</v>
       </c>
       <c r="C199" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D199" t="s">
         <v>6</v>
@@ -3275,7 +3278,7 @@
         <v>13</v>
       </c>
       <c r="C200" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D200" t="s">
         <v>9</v>
@@ -3289,7 +3292,7 @@
         <v>16</v>
       </c>
       <c r="C201" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D201" t="s">
         <v>15</v>
@@ -3303,7 +3306,7 @@
         <v>4</v>
       </c>
       <c r="C202" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D202" t="s">
         <v>6</v>
@@ -3331,7 +3334,7 @@
         <v>10</v>
       </c>
       <c r="C204" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D204" t="s">
         <v>9</v>
@@ -3359,7 +3362,7 @@
         <v>16</v>
       </c>
       <c r="C206" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D206" t="s">
         <v>9</v>
@@ -3401,7 +3404,7 @@
         <v>10</v>
       </c>
       <c r="C209" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D209" t="s">
         <v>15</v>
@@ -3443,7 +3446,7 @@
         <v>4</v>
       </c>
       <c r="C212" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D212" t="s">
         <v>15</v>
@@ -3471,7 +3474,7 @@
         <v>10</v>
       </c>
       <c r="C214" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D214" t="s">
         <v>9</v>
@@ -3499,7 +3502,7 @@
         <v>16</v>
       </c>
       <c r="C216" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D216" t="s">
         <v>12</v>
@@ -3541,7 +3544,7 @@
         <v>10</v>
       </c>
       <c r="C219" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D219" t="s">
         <v>6</v>
@@ -3611,7 +3614,7 @@
         <v>10</v>
       </c>
       <c r="C224" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D224" t="s">
         <v>12</v>
@@ -3625,7 +3628,7 @@
         <v>13</v>
       </c>
       <c r="C225" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D225" t="s">
         <v>12</v>
@@ -3653,7 +3656,7 @@
         <v>4</v>
       </c>
       <c r="C227" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D227" t="s">
         <v>12</v>
@@ -3751,7 +3754,7 @@
         <v>10</v>
       </c>
       <c r="C234" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D234" t="s">
         <v>9</v>
@@ -3765,7 +3768,7 @@
         <v>13</v>
       </c>
       <c r="C235" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D235" t="s">
         <v>15</v>
@@ -3793,7 +3796,7 @@
         <v>4</v>
       </c>
       <c r="C237" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D237" t="s">
         <v>15</v>
@@ -3863,7 +3866,7 @@
         <v>4</v>
       </c>
       <c r="C242" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D242" t="s">
         <v>6</v>
@@ -3891,7 +3894,7 @@
         <v>10</v>
       </c>
       <c r="C244" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D244" t="s">
         <v>15</v>
@@ -3961,7 +3964,7 @@
         <v>10</v>
       </c>
       <c r="C249" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D249" t="s">
         <v>15</v>
@@ -4003,7 +4006,7 @@
         <v>4</v>
       </c>
       <c r="C252" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D252" t="s">
         <v>9</v>
@@ -4031,7 +4034,7 @@
         <v>10</v>
       </c>
       <c r="C254" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D254" t="s">
         <v>15</v>
@@ -4073,7 +4076,7 @@
         <v>4</v>
       </c>
       <c r="C257" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D257" t="s">
         <v>9</v>
@@ -4087,7 +4090,7 @@
         <v>7</v>
       </c>
       <c r="C258" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D258" t="s">
         <v>6</v>
@@ -4101,7 +4104,7 @@
         <v>10</v>
       </c>
       <c r="C259" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D259" t="s">
         <v>15</v>
@@ -4115,7 +4118,7 @@
         <v>13</v>
       </c>
       <c r="C260" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D260" t="s">
         <v>6</v>
@@ -4129,7 +4132,7 @@
         <v>16</v>
       </c>
       <c r="C261" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D261" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
override type added on employee and delete gitkeep
</commit_message>
<xml_diff>
--- a/oppgave_3/files/lunch.xlsx
+++ b/oppgave_3/files/lunch.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="29">
   <si>
     <t>Week Number</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Mandag</t>
   </si>
   <si>
-    <t>Simen</t>
+    <t>Philip</t>
   </si>
   <si>
     <t>Pizza</t>
@@ -52,13 +52,13 @@
     <t>Torsdag</t>
   </si>
   <si>
+    <t>Simen</t>
+  </si>
+  <si>
     <t>Fredag</t>
   </si>
   <si>
     <t>Kaare</t>
-  </si>
-  <si>
-    <t>Fisk</t>
   </si>
   <si>
     <t>Olav</t>
@@ -67,10 +67,10 @@
     <t>Trine</t>
   </si>
   <si>
-    <t>Finn</t>
+    <t>Taco</t>
   </si>
   <si>
-    <t>Taco</t>
+    <t>Finn</t>
   </si>
   <si>
     <t>Oline</t>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Trude</t>
+  </si>
+  <si>
+    <t>Fisk</t>
   </si>
   <si>
     <t>Sharek</t>
@@ -534,7 +537,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -545,10 +548,10 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -556,13 +559,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,7 +593,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -601,10 +604,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -618,7 +621,7 @@
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -626,13 +629,13 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -646,7 +649,7 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -660,7 +663,7 @@
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -674,7 +677,7 @@
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -685,10 +688,10 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -696,13 +699,13 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -716,7 +719,7 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,7 +733,7 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -741,7 +744,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
@@ -758,7 +761,7 @@
         <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -766,7 +769,7 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
         <v>21</v>
@@ -786,7 +789,7 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -797,10 +800,10 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -811,10 +814,10 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -828,7 +831,7 @@
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -836,13 +839,13 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -856,7 +859,7 @@
         <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -870,7 +873,7 @@
         <v>21</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -884,7 +887,7 @@
         <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -895,10 +898,10 @@
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -906,7 +909,7 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
@@ -926,7 +929,7 @@
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -937,10 +940,10 @@
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -951,10 +954,10 @@
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -976,13 +979,13 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D36" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -993,10 +996,10 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1007,10 +1010,10 @@
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1021,7 +1024,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D39" t="s">
         <v>6</v>
@@ -1035,10 +1038,10 @@
         <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,10 +1049,10 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D41" t="s">
         <v>6</v>
@@ -1063,7 +1066,7 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
@@ -1080,7 +1083,7 @@
         <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1091,10 +1094,10 @@
         <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1105,10 +1108,10 @@
         <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D45" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1116,13 +1119,13 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D46" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1136,7 +1139,7 @@
         <v>22</v>
       </c>
       <c r="D47" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,7 +1153,7 @@
         <v>17</v>
       </c>
       <c r="D48" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1164,7 +1167,7 @@
         <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1175,10 +1178,10 @@
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D50" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1186,13 +1189,13 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C51" t="s">
         <v>20</v>
       </c>
       <c r="D51" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1203,10 +1206,10 @@
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D52" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1220,7 +1223,7 @@
         <v>11</v>
       </c>
       <c r="D53" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1231,10 +1234,10 @@
         <v>10</v>
       </c>
       <c r="C54" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D54" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1245,10 +1248,10 @@
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D55" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1256,13 +1259,13 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D56" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1276,7 +1279,7 @@
         <v>22</v>
       </c>
       <c r="D57" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1290,7 +1293,7 @@
         <v>17</v>
       </c>
       <c r="D58" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1304,7 +1307,7 @@
         <v>16</v>
       </c>
       <c r="D59" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1315,7 +1318,7 @@
         <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D60" t="s">
         <v>9</v>
@@ -1326,13 +1329,13 @@
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C61" t="s">
         <v>20</v>
       </c>
       <c r="D61" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1343,10 +1346,10 @@
         <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D62" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1357,10 +1360,10 @@
         <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D63" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1371,10 +1374,10 @@
         <v>10</v>
       </c>
       <c r="C64" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D64" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1385,7 +1388,7 @@
         <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D65" t="s">
         <v>6</v>
@@ -1396,10 +1399,10 @@
         <v>13</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D66" t="s">
         <v>9</v>
@@ -1416,7 +1419,7 @@
         <v>17</v>
       </c>
       <c r="D67" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1430,7 +1433,7 @@
         <v>20</v>
       </c>
       <c r="D68" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1444,7 +1447,7 @@
         <v>8</v>
       </c>
       <c r="D69" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1458,7 +1461,7 @@
         <v>11</v>
       </c>
       <c r="D70" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1466,13 +1469,13 @@
         <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C71" t="s">
         <v>21</v>
       </c>
       <c r="D71" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1483,10 +1486,10 @@
         <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D72" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1497,10 +1500,10 @@
         <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D73" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1511,10 +1514,10 @@
         <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D74" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1525,7 +1528,7 @@
         <v>12</v>
       </c>
       <c r="C75" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D75" t="s">
         <v>9</v>
@@ -1536,10 +1539,10 @@
         <v>15</v>
       </c>
       <c r="B76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C76" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D76" t="s">
         <v>9</v>
@@ -1556,7 +1559,7 @@
         <v>17</v>
       </c>
       <c r="D77" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1570,7 +1573,7 @@
         <v>20</v>
       </c>
       <c r="D78" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1584,7 +1587,7 @@
         <v>8</v>
       </c>
       <c r="D79" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1598,7 +1601,7 @@
         <v>11</v>
       </c>
       <c r="D80" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1606,13 +1609,13 @@
         <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C81" t="s">
         <v>21</v>
       </c>
       <c r="D81" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1623,10 +1626,10 @@
         <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D82" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1637,10 +1640,10 @@
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D83" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1651,10 +1654,10 @@
         <v>10</v>
       </c>
       <c r="C84" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D84" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1676,13 +1679,13 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C86" t="s">
         <v>11</v>
       </c>
       <c r="D86" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1693,10 +1696,10 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D87" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1710,7 +1713,7 @@
         <v>22</v>
       </c>
       <c r="D88" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1724,7 +1727,7 @@
         <v>16</v>
       </c>
       <c r="D89" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1738,7 +1741,7 @@
         <v>20</v>
       </c>
       <c r="D90" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -1746,13 +1749,13 @@
         <v>18</v>
       </c>
       <c r="B91" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C91" t="s">
         <v>21</v>
       </c>
       <c r="D91" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -1763,10 +1766,10 @@
         <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D92" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1777,10 +1780,10 @@
         <v>7</v>
       </c>
       <c r="C93" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D93" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -1791,10 +1794,10 @@
         <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D94" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -1808,7 +1811,7 @@
         <v>8</v>
       </c>
       <c r="D95" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -1816,13 +1819,13 @@
         <v>19</v>
       </c>
       <c r="B96" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C96" t="s">
         <v>11</v>
       </c>
       <c r="D96" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -1833,10 +1836,10 @@
         <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D97" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1850,7 +1853,7 @@
         <v>22</v>
       </c>
       <c r="D98" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1878,7 +1881,7 @@
         <v>20</v>
       </c>
       <c r="D100" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -1886,13 +1889,13 @@
         <v>20</v>
       </c>
       <c r="B101" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C101" t="s">
         <v>21</v>
       </c>
       <c r="D101" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -1903,10 +1906,10 @@
         <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D102" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -1917,7 +1920,7 @@
         <v>7</v>
       </c>
       <c r="C103" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D103" t="s">
         <v>6</v>
@@ -1934,7 +1937,7 @@
         <v>8</v>
       </c>
       <c r="D104" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -1945,7 +1948,7 @@
         <v>12</v>
       </c>
       <c r="C105" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D105" t="s">
         <v>9</v>
@@ -1956,13 +1959,13 @@
         <v>21</v>
       </c>
       <c r="B106" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C106" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D106" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -1976,7 +1979,7 @@
         <v>22</v>
       </c>
       <c r="D107" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -1990,7 +1993,7 @@
         <v>21</v>
       </c>
       <c r="D108" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2004,7 +2007,7 @@
         <v>20</v>
       </c>
       <c r="D109" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2015,10 +2018,10 @@
         <v>12</v>
       </c>
       <c r="C110" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D110" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2026,13 +2029,13 @@
         <v>22</v>
       </c>
       <c r="B111" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C111" t="s">
         <v>16</v>
       </c>
       <c r="D111" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2043,10 +2046,10 @@
         <v>4</v>
       </c>
       <c r="C112" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D112" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2057,10 +2060,10 @@
         <v>7</v>
       </c>
       <c r="C113" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D113" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2085,10 +2088,10 @@
         <v>12</v>
       </c>
       <c r="C115" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D115" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2096,13 +2099,13 @@
         <v>23</v>
       </c>
       <c r="B116" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C116" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D116" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2116,7 +2119,7 @@
         <v>22</v>
       </c>
       <c r="D117" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2130,7 +2133,7 @@
         <v>21</v>
       </c>
       <c r="D118" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2144,7 +2147,7 @@
         <v>20</v>
       </c>
       <c r="D119" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2155,10 +2158,10 @@
         <v>12</v>
       </c>
       <c r="C120" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D120" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2166,13 +2169,13 @@
         <v>24</v>
       </c>
       <c r="B121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C121" t="s">
         <v>16</v>
       </c>
       <c r="D121" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2186,7 +2189,7 @@
         <v>16</v>
       </c>
       <c r="D122" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2197,7 +2200,7 @@
         <v>7</v>
       </c>
       <c r="C123" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D123" t="s">
         <v>6</v>
@@ -2214,7 +2217,7 @@
         <v>11</v>
       </c>
       <c r="D124" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2225,10 +2228,10 @@
         <v>12</v>
       </c>
       <c r="C125" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D125" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -2236,13 +2239,13 @@
         <v>25</v>
       </c>
       <c r="B126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C126" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D126" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2256,7 +2259,7 @@
         <v>8</v>
       </c>
       <c r="D127" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -2270,7 +2273,7 @@
         <v>22</v>
       </c>
       <c r="D128" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -2284,7 +2287,7 @@
         <v>21</v>
       </c>
       <c r="D129" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -2295,10 +2298,10 @@
         <v>12</v>
       </c>
       <c r="C130" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D130" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -2306,13 +2309,13 @@
         <v>26</v>
       </c>
       <c r="B131" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C131" t="s">
         <v>20</v>
       </c>
       <c r="D131" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2326,7 +2329,7 @@
         <v>16</v>
       </c>
       <c r="D132" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -2337,10 +2340,10 @@
         <v>7</v>
       </c>
       <c r="C133" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D133" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -2354,7 +2357,7 @@
         <v>11</v>
       </c>
       <c r="D134" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -2365,10 +2368,10 @@
         <v>12</v>
       </c>
       <c r="C135" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D135" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -2376,13 +2379,13 @@
         <v>27</v>
       </c>
       <c r="B136" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C136" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D136" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -2393,10 +2396,10 @@
         <v>4</v>
       </c>
       <c r="C137" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D137" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -2407,10 +2410,10 @@
         <v>7</v>
       </c>
       <c r="C138" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D138" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -2421,10 +2424,10 @@
         <v>10</v>
       </c>
       <c r="C139" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D139" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -2435,10 +2438,10 @@
         <v>12</v>
       </c>
       <c r="C140" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D140" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -2446,10 +2449,10 @@
         <v>28</v>
       </c>
       <c r="B141" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C141" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D141" t="s">
         <v>6</v>
@@ -2463,10 +2466,10 @@
         <v>4</v>
       </c>
       <c r="C142" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D142" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -2477,10 +2480,10 @@
         <v>7</v>
       </c>
       <c r="C143" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D143" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -2491,10 +2494,10 @@
         <v>10</v>
       </c>
       <c r="C144" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D144" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -2505,10 +2508,10 @@
         <v>12</v>
       </c>
       <c r="C145" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D145" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -2516,13 +2519,13 @@
         <v>29</v>
       </c>
       <c r="B146" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C146" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D146" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -2533,10 +2536,10 @@
         <v>4</v>
       </c>
       <c r="C147" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D147" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -2547,7 +2550,7 @@
         <v>7</v>
       </c>
       <c r="C148" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D148" t="s">
         <v>6</v>
@@ -2561,7 +2564,7 @@
         <v>10</v>
       </c>
       <c r="C149" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D149" t="s">
         <v>9</v>
@@ -2575,10 +2578,10 @@
         <v>12</v>
       </c>
       <c r="C150" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D150" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -2586,10 +2589,10 @@
         <v>30</v>
       </c>
       <c r="B151" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C151" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D151" t="s">
         <v>9</v>
@@ -2603,10 +2606,10 @@
         <v>4</v>
       </c>
       <c r="C152" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D152" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -2617,10 +2620,10 @@
         <v>7</v>
       </c>
       <c r="C153" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D153" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -2631,10 +2634,10 @@
         <v>10</v>
       </c>
       <c r="C154" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D154" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -2645,10 +2648,10 @@
         <v>12</v>
       </c>
       <c r="C155" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D155" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -2656,13 +2659,13 @@
         <v>31</v>
       </c>
       <c r="B156" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C156" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D156" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -2673,10 +2676,10 @@
         <v>4</v>
       </c>
       <c r="C157" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D157" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -2687,10 +2690,10 @@
         <v>7</v>
       </c>
       <c r="C158" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D158" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -2701,10 +2704,10 @@
         <v>10</v>
       </c>
       <c r="C159" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D159" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -2715,10 +2718,10 @@
         <v>12</v>
       </c>
       <c r="C160" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D160" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -2726,13 +2729,13 @@
         <v>32</v>
       </c>
       <c r="B161" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C161" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D161" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -2743,10 +2746,10 @@
         <v>4</v>
       </c>
       <c r="C162" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D162" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -2757,10 +2760,10 @@
         <v>7</v>
       </c>
       <c r="C163" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D163" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -2771,10 +2774,10 @@
         <v>10</v>
       </c>
       <c r="C164" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D164" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -2785,10 +2788,10 @@
         <v>12</v>
       </c>
       <c r="C165" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D165" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -2796,13 +2799,13 @@
         <v>33</v>
       </c>
       <c r="B166" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C166" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D166" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -2816,7 +2819,7 @@
         <v>20</v>
       </c>
       <c r="D167" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -2830,7 +2833,7 @@
         <v>22</v>
       </c>
       <c r="D168" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -2844,7 +2847,7 @@
         <v>21</v>
       </c>
       <c r="D169" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -2855,10 +2858,10 @@
         <v>12</v>
       </c>
       <c r="C170" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D170" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -2866,13 +2869,13 @@
         <v>34</v>
       </c>
       <c r="B171" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C171" t="s">
         <v>8</v>
       </c>
       <c r="D171" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -2883,10 +2886,10 @@
         <v>4</v>
       </c>
       <c r="C172" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D172" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -2897,10 +2900,10 @@
         <v>7</v>
       </c>
       <c r="C173" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D173" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -2911,7 +2914,7 @@
         <v>10</v>
       </c>
       <c r="C174" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D174" t="s">
         <v>9</v>
@@ -2925,10 +2928,10 @@
         <v>12</v>
       </c>
       <c r="C175" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D175" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -2936,10 +2939,10 @@
         <v>35</v>
       </c>
       <c r="B176" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C176" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D176" t="s">
         <v>9</v>
@@ -2956,7 +2959,7 @@
         <v>20</v>
       </c>
       <c r="D177" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -2970,7 +2973,7 @@
         <v>22</v>
       </c>
       <c r="D178" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -2984,7 +2987,7 @@
         <v>21</v>
       </c>
       <c r="D179" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -2995,10 +2998,10 @@
         <v>12</v>
       </c>
       <c r="C180" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D180" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -3006,13 +3009,13 @@
         <v>36</v>
       </c>
       <c r="B181" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C181" t="s">
         <v>8</v>
       </c>
       <c r="D181" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -3037,10 +3040,10 @@
         <v>7</v>
       </c>
       <c r="C183" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D183" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -3051,10 +3054,10 @@
         <v>10</v>
       </c>
       <c r="C184" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D184" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -3065,10 +3068,10 @@
         <v>12</v>
       </c>
       <c r="C185" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D185" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -3076,13 +3079,13 @@
         <v>37</v>
       </c>
       <c r="B186" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C186" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D186" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -3096,7 +3099,7 @@
         <v>22</v>
       </c>
       <c r="D187" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -3110,7 +3113,7 @@
         <v>16</v>
       </c>
       <c r="D188" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -3124,7 +3127,7 @@
         <v>11</v>
       </c>
       <c r="D189" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -3135,10 +3138,10 @@
         <v>12</v>
       </c>
       <c r="C190" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D190" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -3146,13 +3149,13 @@
         <v>38</v>
       </c>
       <c r="B191" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C191" t="s">
         <v>20</v>
       </c>
       <c r="D191" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -3166,7 +3169,7 @@
         <v>8</v>
       </c>
       <c r="D192" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -3177,10 +3180,10 @@
         <v>7</v>
       </c>
       <c r="C193" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D193" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -3191,10 +3194,10 @@
         <v>10</v>
       </c>
       <c r="C194" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D194" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -3205,10 +3208,10 @@
         <v>12</v>
       </c>
       <c r="C195" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D195" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -3216,13 +3219,13 @@
         <v>39</v>
       </c>
       <c r="B196" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C196" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D196" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -3233,10 +3236,10 @@
         <v>4</v>
       </c>
       <c r="C197" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D197" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -3247,10 +3250,10 @@
         <v>7</v>
       </c>
       <c r="C198" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D198" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -3261,10 +3264,10 @@
         <v>10</v>
       </c>
       <c r="C199" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D199" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -3275,10 +3278,10 @@
         <v>12</v>
       </c>
       <c r="C200" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D200" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -3286,13 +3289,13 @@
         <v>40</v>
       </c>
       <c r="B201" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C201" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D201" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -3303,10 +3306,10 @@
         <v>4</v>
       </c>
       <c r="C202" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D202" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -3317,7 +3320,7 @@
         <v>7</v>
       </c>
       <c r="C203" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D203" t="s">
         <v>9</v>
@@ -3331,7 +3334,7 @@
         <v>10</v>
       </c>
       <c r="C204" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D204" t="s">
         <v>6</v>
@@ -3348,7 +3351,7 @@
         <v>11</v>
       </c>
       <c r="D205" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -3356,13 +3359,13 @@
         <v>41</v>
       </c>
       <c r="B206" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C206" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D206" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -3376,7 +3379,7 @@
         <v>8</v>
       </c>
       <c r="D207" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -3390,7 +3393,7 @@
         <v>16</v>
       </c>
       <c r="D208" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -3401,10 +3404,10 @@
         <v>10</v>
       </c>
       <c r="C209" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D209" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -3415,10 +3418,10 @@
         <v>12</v>
       </c>
       <c r="C210" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D210" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -3426,13 +3429,13 @@
         <v>42</v>
       </c>
       <c r="B211" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C211" t="s">
         <v>21</v>
       </c>
       <c r="D211" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -3443,10 +3446,10 @@
         <v>4</v>
       </c>
       <c r="C212" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D212" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -3457,10 +3460,10 @@
         <v>7</v>
       </c>
       <c r="C213" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D213" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -3471,7 +3474,7 @@
         <v>10</v>
       </c>
       <c r="C214" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D214" t="s">
         <v>6</v>
@@ -3488,7 +3491,7 @@
         <v>11</v>
       </c>
       <c r="D215" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -3496,13 +3499,13 @@
         <v>43</v>
       </c>
       <c r="B216" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C216" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D216" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -3516,7 +3519,7 @@
         <v>8</v>
       </c>
       <c r="D217" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -3530,7 +3533,7 @@
         <v>16</v>
       </c>
       <c r="D218" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -3541,10 +3544,10 @@
         <v>10</v>
       </c>
       <c r="C219" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D219" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -3555,10 +3558,10 @@
         <v>12</v>
       </c>
       <c r="C220" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D220" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -3566,13 +3569,13 @@
         <v>44</v>
       </c>
       <c r="B221" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C221" t="s">
         <v>21</v>
       </c>
       <c r="D221" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -3586,7 +3589,7 @@
         <v>11</v>
       </c>
       <c r="D222" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -3597,10 +3600,10 @@
         <v>7</v>
       </c>
       <c r="C223" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D223" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -3611,10 +3614,10 @@
         <v>10</v>
       </c>
       <c r="C224" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D224" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -3625,10 +3628,10 @@
         <v>12</v>
       </c>
       <c r="C225" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D225" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -3636,10 +3639,10 @@
         <v>45</v>
       </c>
       <c r="B226" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C226" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D226" t="s">
         <v>9</v>
@@ -3656,7 +3659,7 @@
         <v>22</v>
       </c>
       <c r="D227" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -3667,10 +3670,10 @@
         <v>7</v>
       </c>
       <c r="C228" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D228" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -3684,7 +3687,7 @@
         <v>21</v>
       </c>
       <c r="D229" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -3698,7 +3701,7 @@
         <v>20</v>
       </c>
       <c r="D230" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -3706,13 +3709,13 @@
         <v>46</v>
       </c>
       <c r="B231" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C231" t="s">
         <v>16</v>
       </c>
       <c r="D231" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -3726,7 +3729,7 @@
         <v>11</v>
       </c>
       <c r="D232" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -3737,10 +3740,10 @@
         <v>7</v>
       </c>
       <c r="C233" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D233" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -3751,7 +3754,7 @@
         <v>10</v>
       </c>
       <c r="C234" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D234" t="s">
         <v>9</v>
@@ -3765,10 +3768,10 @@
         <v>12</v>
       </c>
       <c r="C235" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D235" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -3776,13 +3779,13 @@
         <v>47</v>
       </c>
       <c r="B236" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C236" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D236" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -3796,7 +3799,7 @@
         <v>22</v>
       </c>
       <c r="D237" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
@@ -3807,7 +3810,7 @@
         <v>7</v>
       </c>
       <c r="C238" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D238" t="s">
         <v>9</v>
@@ -3824,7 +3827,7 @@
         <v>21</v>
       </c>
       <c r="D239" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -3838,7 +3841,7 @@
         <v>20</v>
       </c>
       <c r="D240" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -3846,13 +3849,13 @@
         <v>48</v>
       </c>
       <c r="B241" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C241" t="s">
         <v>16</v>
       </c>
       <c r="D241" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -3863,10 +3866,10 @@
         <v>4</v>
       </c>
       <c r="C242" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D242" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -3877,10 +3880,10 @@
         <v>7</v>
       </c>
       <c r="C243" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D243" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -3891,10 +3894,10 @@
         <v>10</v>
       </c>
       <c r="C244" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D244" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -3905,10 +3908,10 @@
         <v>12</v>
       </c>
       <c r="C245" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D245" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -3916,13 +3919,13 @@
         <v>49</v>
       </c>
       <c r="B246" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C246" t="s">
         <v>8</v>
       </c>
       <c r="D246" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -3936,7 +3939,7 @@
         <v>11</v>
       </c>
       <c r="D247" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -3950,7 +3953,7 @@
         <v>17</v>
       </c>
       <c r="D248" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -3964,7 +3967,7 @@
         <v>22</v>
       </c>
       <c r="D249" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -3975,10 +3978,10 @@
         <v>12</v>
       </c>
       <c r="C250" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D250" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -3986,13 +3989,13 @@
         <v>50</v>
       </c>
       <c r="B251" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C251" t="s">
         <v>20</v>
       </c>
       <c r="D251" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -4003,7 +4006,7 @@
         <v>4</v>
       </c>
       <c r="C252" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D252" t="s">
         <v>9</v>
@@ -4017,10 +4020,10 @@
         <v>7</v>
       </c>
       <c r="C253" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D253" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
@@ -4031,10 +4034,10 @@
         <v>10</v>
       </c>
       <c r="C254" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D254" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -4045,10 +4048,10 @@
         <v>12</v>
       </c>
       <c r="C255" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D255" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -4056,13 +4059,13 @@
         <v>51</v>
       </c>
       <c r="B256" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C256" t="s">
         <v>8</v>
       </c>
       <c r="D256" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -4073,10 +4076,10 @@
         <v>4</v>
       </c>
       <c r="C257" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D257" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -4087,10 +4090,10 @@
         <v>7</v>
       </c>
       <c r="C258" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D258" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -4101,10 +4104,10 @@
         <v>10</v>
       </c>
       <c r="C259" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D259" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -4115,10 +4118,10 @@
         <v>12</v>
       </c>
       <c r="C260" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D260" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -4126,13 +4129,13 @@
         <v>52</v>
       </c>
       <c r="B261" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C261" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D261" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some small changes with excel api
</commit_message>
<xml_diff>
--- a/oppgave_3/files/lunch.xlsx
+++ b/oppgave_3/files/lunch.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="28">
   <si>
     <t>Week Number</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Mandag</t>
   </si>
   <si>
-    <t>Philip</t>
+    <t>Trude</t>
   </si>
   <si>
     <t>Pizza</t>
@@ -49,6 +49,9 @@
     <t>Lars</t>
   </si>
   <si>
+    <t>Taco</t>
+  </si>
+  <si>
     <t>Torsdag</t>
   </si>
   <si>
@@ -61,13 +64,13 @@
     <t>Kaare</t>
   </si>
   <si>
+    <t>Fisk</t>
+  </si>
+  <si>
     <t>Olav</t>
   </si>
   <si>
     <t>Trine</t>
-  </si>
-  <si>
-    <t>Taco</t>
   </si>
   <si>
     <t>Finn</t>
@@ -77,12 +80,6 @@
   </si>
   <si>
     <t>Nora</t>
-  </si>
-  <si>
-    <t>Trude</t>
-  </si>
-  <si>
-    <t>Fisk</t>
   </si>
   <si>
     <t>Sharek</t>
@@ -537,7 +534,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -545,13 +542,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -559,13 +556,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -576,10 +573,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,10 +587,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -604,10 +601,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -615,13 +612,13 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -629,13 +626,13 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -646,10 +643,10 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,7 +660,7 @@
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -677,7 +674,7 @@
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -685,10 +682,10 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -699,13 +696,13 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -716,7 +713,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
@@ -730,10 +727,10 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -744,10 +741,10 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -755,13 +752,13 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -769,13 +766,13 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -786,10 +783,10 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -800,10 +797,10 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -814,10 +811,10 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -825,13 +822,13 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,13 +836,13 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -856,10 +853,10 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -870,7 +867,7 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
@@ -884,10 +881,10 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -895,10 +892,10 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
@@ -909,13 +906,13 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -926,10 +923,10 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -940,10 +937,10 @@
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -954,10 +951,10 @@
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -965,13 +962,13 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -979,10 +976,10 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
@@ -996,10 +993,10 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1010,10 +1007,10 @@
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1024,7 +1021,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D39" t="s">
         <v>6</v>
@@ -1035,13 +1032,13 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D40" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1049,13 +1046,13 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1066,10 +1063,10 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1083,7 +1080,7 @@
         <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1094,10 +1091,10 @@
         <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D44" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1105,13 +1102,13 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D45" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1119,10 +1116,10 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D46" t="s">
         <v>9</v>
@@ -1136,10 +1133,10 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,10 +1147,10 @@
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D48" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1164,10 +1161,10 @@
         <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1175,13 +1172,13 @@
         <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D50" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1189,10 +1186,10 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C51" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D51" t="s">
         <v>9</v>
@@ -1206,7 +1203,7 @@
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D52" t="s">
         <v>9</v>
@@ -1223,7 +1220,7 @@
         <v>11</v>
       </c>
       <c r="D53" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1234,10 +1231,10 @@
         <v>10</v>
       </c>
       <c r="C54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D54" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1245,10 +1242,10 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D55" t="s">
         <v>6</v>
@@ -1259,13 +1256,13 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C56" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D56" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1276,10 +1273,10 @@
         <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D57" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1290,10 +1287,10 @@
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D58" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1304,10 +1301,10 @@
         <v>10</v>
       </c>
       <c r="C59" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1315,13 +1312,13 @@
         <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D60" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1329,13 +1326,13 @@
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D61" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1346,10 +1343,10 @@
         <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D62" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1360,7 +1357,7 @@
         <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D63" t="s">
         <v>6</v>
@@ -1374,10 +1371,10 @@
         <v>10</v>
       </c>
       <c r="C64" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1385,13 +1382,13 @@
         <v>13</v>
       </c>
       <c r="B65" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C65" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D65" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1399,13 +1396,13 @@
         <v>13</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C66" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1416,10 +1413,10 @@
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D67" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1430,7 +1427,7 @@
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D68" t="s">
         <v>6</v>
@@ -1447,7 +1444,7 @@
         <v>8</v>
       </c>
       <c r="D69" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1455,13 +1452,13 @@
         <v>14</v>
       </c>
       <c r="B70" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C70" t="s">
         <v>11</v>
       </c>
       <c r="D70" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1469,13 +1466,13 @@
         <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C71" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D71" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1486,10 +1483,10 @@
         <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D72" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1500,10 +1497,10 @@
         <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D73" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1514,10 +1511,10 @@
         <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D74" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1525,13 +1522,13 @@
         <v>15</v>
       </c>
       <c r="B75" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C75" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D75" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1539,13 +1536,13 @@
         <v>15</v>
       </c>
       <c r="B76" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C76" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D76" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1556,10 +1553,10 @@
         <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D77" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1570,10 +1567,10 @@
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D78" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1587,7 +1584,7 @@
         <v>8</v>
       </c>
       <c r="D79" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1595,13 +1592,13 @@
         <v>16</v>
       </c>
       <c r="B80" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C80" t="s">
         <v>11</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1609,13 +1606,13 @@
         <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C81" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D81" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1626,10 +1623,10 @@
         <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D82" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1640,10 +1637,10 @@
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D83" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1654,10 +1651,10 @@
         <v>10</v>
       </c>
       <c r="C84" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D84" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1665,7 +1662,7 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
@@ -1679,13 +1676,13 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C86" t="s">
         <v>11</v>
       </c>
       <c r="D86" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1696,10 +1693,10 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D87" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1710,7 +1707,7 @@
         <v>7</v>
       </c>
       <c r="C88" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D88" t="s">
         <v>9</v>
@@ -1724,10 +1721,10 @@
         <v>10</v>
       </c>
       <c r="C89" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D89" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1735,13 +1732,13 @@
         <v>18</v>
       </c>
       <c r="B90" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C90" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D90" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -1749,13 +1746,13 @@
         <v>18</v>
       </c>
       <c r="B91" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C91" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D91" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -1766,10 +1763,10 @@
         <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D92" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1780,10 +1777,10 @@
         <v>7</v>
       </c>
       <c r="C93" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D93" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -1794,10 +1791,10 @@
         <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D94" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -1805,13 +1802,13 @@
         <v>19</v>
       </c>
       <c r="B95" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C95" t="s">
         <v>8</v>
       </c>
       <c r="D95" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -1819,13 +1816,13 @@
         <v>19</v>
       </c>
       <c r="B96" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C96" t="s">
         <v>11</v>
       </c>
       <c r="D96" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -1836,10 +1833,10 @@
         <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D97" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1850,10 +1847,10 @@
         <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D98" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1864,10 +1861,10 @@
         <v>10</v>
       </c>
       <c r="C99" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D99" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -1875,10 +1872,10 @@
         <v>20</v>
       </c>
       <c r="B100" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C100" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D100" t="s">
         <v>6</v>
@@ -1889,10 +1886,10 @@
         <v>20</v>
       </c>
       <c r="B101" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C101" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D101" t="s">
         <v>9</v>
@@ -1906,10 +1903,10 @@
         <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D102" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -1920,10 +1917,10 @@
         <v>7</v>
       </c>
       <c r="C103" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D103" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -1937,7 +1934,7 @@
         <v>8</v>
       </c>
       <c r="D104" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -1945,13 +1942,13 @@
         <v>21</v>
       </c>
       <c r="B105" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C105" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D105" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -1959,13 +1956,13 @@
         <v>21</v>
       </c>
       <c r="B106" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C106" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D106" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -1976,10 +1973,10 @@
         <v>4</v>
       </c>
       <c r="C107" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D107" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -1990,7 +1987,7 @@
         <v>7</v>
       </c>
       <c r="C108" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D108" t="s">
         <v>9</v>
@@ -2004,10 +2001,10 @@
         <v>10</v>
       </c>
       <c r="C109" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D109" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2015,13 +2012,13 @@
         <v>22</v>
       </c>
       <c r="B110" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C110" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D110" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2029,13 +2026,13 @@
         <v>22</v>
       </c>
       <c r="B111" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C111" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D111" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2046,10 +2043,10 @@
         <v>4</v>
       </c>
       <c r="C112" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D112" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2060,10 +2057,10 @@
         <v>7</v>
       </c>
       <c r="C113" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D113" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2077,7 +2074,7 @@
         <v>8</v>
       </c>
       <c r="D114" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2085,13 +2082,13 @@
         <v>23</v>
       </c>
       <c r="B115" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C115" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D115" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2099,13 +2096,13 @@
         <v>23</v>
       </c>
       <c r="B116" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C116" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D116" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2116,10 +2113,10 @@
         <v>4</v>
       </c>
       <c r="C117" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D117" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2130,10 +2127,10 @@
         <v>7</v>
       </c>
       <c r="C118" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D118" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2144,10 +2141,10 @@
         <v>10</v>
       </c>
       <c r="C119" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D119" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2155,13 +2152,13 @@
         <v>24</v>
       </c>
       <c r="B120" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C120" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D120" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2169,13 +2166,13 @@
         <v>24</v>
       </c>
       <c r="B121" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C121" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D121" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2186,10 +2183,10 @@
         <v>4</v>
       </c>
       <c r="C122" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D122" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2200,10 +2197,10 @@
         <v>7</v>
       </c>
       <c r="C123" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D123" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2217,7 +2214,7 @@
         <v>11</v>
       </c>
       <c r="D124" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2225,13 +2222,13 @@
         <v>25</v>
       </c>
       <c r="B125" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C125" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D125" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -2239,13 +2236,13 @@
         <v>25</v>
       </c>
       <c r="B126" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C126" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D126" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,7 +2256,7 @@
         <v>8</v>
       </c>
       <c r="D127" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -2270,7 +2267,7 @@
         <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D128" t="s">
         <v>6</v>
@@ -2284,10 +2281,10 @@
         <v>10</v>
       </c>
       <c r="C129" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D129" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -2295,10 +2292,10 @@
         <v>26</v>
       </c>
       <c r="B130" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C130" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D130" t="s">
         <v>9</v>
@@ -2309,13 +2306,13 @@
         <v>26</v>
       </c>
       <c r="B131" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C131" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D131" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2326,10 +2323,10 @@
         <v>4</v>
       </c>
       <c r="C132" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D132" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -2340,10 +2337,10 @@
         <v>7</v>
       </c>
       <c r="C133" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D133" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -2357,7 +2354,7 @@
         <v>11</v>
       </c>
       <c r="D134" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -2365,13 +2362,13 @@
         <v>27</v>
       </c>
       <c r="B135" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C135" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D135" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -2379,10 +2376,10 @@
         <v>27</v>
       </c>
       <c r="B136" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C136" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D136" t="s">
         <v>6</v>
@@ -2396,10 +2393,10 @@
         <v>4</v>
       </c>
       <c r="C137" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D137" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -2410,10 +2407,10 @@
         <v>7</v>
       </c>
       <c r="C138" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D138" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -2424,10 +2421,10 @@
         <v>10</v>
       </c>
       <c r="C139" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D139" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -2435,13 +2432,13 @@
         <v>28</v>
       </c>
       <c r="B140" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C140" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D140" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -2449,10 +2446,10 @@
         <v>28</v>
       </c>
       <c r="B141" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C141" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D141" t="s">
         <v>6</v>
@@ -2466,10 +2463,10 @@
         <v>4</v>
       </c>
       <c r="C142" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D142" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -2480,10 +2477,10 @@
         <v>7</v>
       </c>
       <c r="C143" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D143" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -2494,10 +2491,10 @@
         <v>10</v>
       </c>
       <c r="C144" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D144" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -2505,13 +2502,13 @@
         <v>29</v>
       </c>
       <c r="B145" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C145" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D145" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -2519,13 +2516,13 @@
         <v>29</v>
       </c>
       <c r="B146" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C146" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D146" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -2536,10 +2533,10 @@
         <v>4</v>
       </c>
       <c r="C147" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D147" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -2550,10 +2547,10 @@
         <v>7</v>
       </c>
       <c r="C148" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D148" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -2564,10 +2561,10 @@
         <v>10</v>
       </c>
       <c r="C149" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D149" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -2575,13 +2572,13 @@
         <v>30</v>
       </c>
       <c r="B150" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C150" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D150" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -2589,13 +2586,13 @@
         <v>30</v>
       </c>
       <c r="B151" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C151" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D151" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -2606,10 +2603,10 @@
         <v>4</v>
       </c>
       <c r="C152" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D152" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -2620,10 +2617,10 @@
         <v>7</v>
       </c>
       <c r="C153" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D153" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -2634,10 +2631,10 @@
         <v>10</v>
       </c>
       <c r="C154" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D154" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -2645,13 +2642,13 @@
         <v>31</v>
       </c>
       <c r="B155" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C155" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D155" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -2659,13 +2656,13 @@
         <v>31</v>
       </c>
       <c r="B156" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C156" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D156" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -2676,10 +2673,10 @@
         <v>4</v>
       </c>
       <c r="C157" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D157" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -2690,10 +2687,10 @@
         <v>7</v>
       </c>
       <c r="C158" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D158" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -2704,10 +2701,10 @@
         <v>10</v>
       </c>
       <c r="C159" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D159" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -2715,13 +2712,13 @@
         <v>32</v>
       </c>
       <c r="B160" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C160" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D160" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -2729,13 +2726,13 @@
         <v>32</v>
       </c>
       <c r="B161" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C161" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D161" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -2746,10 +2743,10 @@
         <v>4</v>
       </c>
       <c r="C162" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D162" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -2760,10 +2757,10 @@
         <v>7</v>
       </c>
       <c r="C163" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D163" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -2774,10 +2771,10 @@
         <v>10</v>
       </c>
       <c r="C164" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D164" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -2785,13 +2782,13 @@
         <v>33</v>
       </c>
       <c r="B165" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C165" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D165" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -2799,13 +2796,13 @@
         <v>33</v>
       </c>
       <c r="B166" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C166" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D166" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -2816,10 +2813,10 @@
         <v>4</v>
       </c>
       <c r="C167" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D167" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -2830,10 +2827,10 @@
         <v>7</v>
       </c>
       <c r="C168" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D168" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -2844,10 +2841,10 @@
         <v>10</v>
       </c>
       <c r="C169" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D169" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -2855,13 +2852,13 @@
         <v>34</v>
       </c>
       <c r="B170" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D170" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -2869,13 +2866,13 @@
         <v>34</v>
       </c>
       <c r="B171" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C171" t="s">
         <v>8</v>
       </c>
       <c r="D171" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -2886,10 +2883,10 @@
         <v>4</v>
       </c>
       <c r="C172" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D172" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -2900,10 +2897,10 @@
         <v>7</v>
       </c>
       <c r="C173" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D173" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -2914,10 +2911,10 @@
         <v>10</v>
       </c>
       <c r="C174" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D174" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -2925,13 +2922,13 @@
         <v>35</v>
       </c>
       <c r="B175" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C175" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D175" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -2939,10 +2936,10 @@
         <v>35</v>
       </c>
       <c r="B176" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C176" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D176" t="s">
         <v>9</v>
@@ -2956,10 +2953,10 @@
         <v>4</v>
       </c>
       <c r="C177" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D177" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -2970,10 +2967,10 @@
         <v>7</v>
       </c>
       <c r="C178" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D178" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -2984,10 +2981,10 @@
         <v>10</v>
       </c>
       <c r="C179" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D179" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -2995,13 +2992,13 @@
         <v>36</v>
       </c>
       <c r="B180" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C180" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D180" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -3009,13 +3006,13 @@
         <v>36</v>
       </c>
       <c r="B181" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C181" t="s">
         <v>8</v>
       </c>
       <c r="D181" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -3029,7 +3026,7 @@
         <v>8</v>
       </c>
       <c r="D182" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -3040,10 +3037,10 @@
         <v>7</v>
       </c>
       <c r="C183" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D183" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -3054,10 +3051,10 @@
         <v>10</v>
       </c>
       <c r="C184" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D184" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -3065,13 +3062,13 @@
         <v>37</v>
       </c>
       <c r="B185" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C185" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D185" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -3079,13 +3076,13 @@
         <v>37</v>
       </c>
       <c r="B186" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C186" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D186" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -3096,7 +3093,7 @@
         <v>4</v>
       </c>
       <c r="C187" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D187" t="s">
         <v>9</v>
@@ -3110,10 +3107,10 @@
         <v>7</v>
       </c>
       <c r="C188" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D188" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -3127,7 +3124,7 @@
         <v>11</v>
       </c>
       <c r="D189" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -3135,13 +3132,13 @@
         <v>38</v>
       </c>
       <c r="B190" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C190" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D190" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -3149,13 +3146,13 @@
         <v>38</v>
       </c>
       <c r="B191" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C191" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D191" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -3180,10 +3177,10 @@
         <v>7</v>
       </c>
       <c r="C193" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D193" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -3194,10 +3191,10 @@
         <v>10</v>
       </c>
       <c r="C194" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D194" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -3205,13 +3202,13 @@
         <v>39</v>
       </c>
       <c r="B195" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C195" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D195" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -3219,13 +3216,13 @@
         <v>39</v>
       </c>
       <c r="B196" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C196" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D196" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -3236,10 +3233,10 @@
         <v>4</v>
       </c>
       <c r="C197" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D197" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -3250,10 +3247,10 @@
         <v>7</v>
       </c>
       <c r="C198" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D198" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -3264,10 +3261,10 @@
         <v>10</v>
       </c>
       <c r="C199" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D199" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -3275,13 +3272,13 @@
         <v>40</v>
       </c>
       <c r="B200" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C200" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D200" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -3289,13 +3286,13 @@
         <v>40</v>
       </c>
       <c r="B201" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C201" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D201" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -3306,10 +3303,10 @@
         <v>4</v>
       </c>
       <c r="C202" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D202" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -3320,7 +3317,7 @@
         <v>7</v>
       </c>
       <c r="C203" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D203" t="s">
         <v>9</v>
@@ -3334,10 +3331,10 @@
         <v>10</v>
       </c>
       <c r="C204" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D204" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -3345,13 +3342,13 @@
         <v>41</v>
       </c>
       <c r="B205" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C205" t="s">
         <v>11</v>
       </c>
       <c r="D205" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -3359,13 +3356,13 @@
         <v>41</v>
       </c>
       <c r="B206" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C206" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D206" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -3379,7 +3376,7 @@
         <v>8</v>
       </c>
       <c r="D207" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -3390,10 +3387,10 @@
         <v>7</v>
       </c>
       <c r="C208" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D208" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -3404,10 +3401,10 @@
         <v>10</v>
       </c>
       <c r="C209" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D209" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -3415,13 +3412,13 @@
         <v>42</v>
       </c>
       <c r="B210" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C210" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D210" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -3429,13 +3426,13 @@
         <v>42</v>
       </c>
       <c r="B211" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C211" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D211" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -3446,10 +3443,10 @@
         <v>4</v>
       </c>
       <c r="C212" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D212" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -3460,10 +3457,10 @@
         <v>7</v>
       </c>
       <c r="C213" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D213" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -3474,10 +3471,10 @@
         <v>10</v>
       </c>
       <c r="C214" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D214" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -3485,13 +3482,13 @@
         <v>43</v>
       </c>
       <c r="B215" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C215" t="s">
         <v>11</v>
       </c>
       <c r="D215" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -3499,13 +3496,13 @@
         <v>43</v>
       </c>
       <c r="B216" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C216" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D216" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -3519,7 +3516,7 @@
         <v>8</v>
       </c>
       <c r="D217" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -3530,7 +3527,7 @@
         <v>7</v>
       </c>
       <c r="C218" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D218" t="s">
         <v>6</v>
@@ -3544,10 +3541,10 @@
         <v>10</v>
       </c>
       <c r="C219" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D219" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -3555,13 +3552,13 @@
         <v>44</v>
       </c>
       <c r="B220" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C220" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D220" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -3569,13 +3566,13 @@
         <v>44</v>
       </c>
       <c r="B221" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C221" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D221" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -3589,7 +3586,7 @@
         <v>11</v>
       </c>
       <c r="D222" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -3600,10 +3597,10 @@
         <v>7</v>
       </c>
       <c r="C223" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D223" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -3614,10 +3611,10 @@
         <v>10</v>
       </c>
       <c r="C224" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D224" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -3625,13 +3622,13 @@
         <v>45</v>
       </c>
       <c r="B225" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C225" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D225" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -3639,13 +3636,13 @@
         <v>45</v>
       </c>
       <c r="B226" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C226" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D226" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -3656,10 +3653,10 @@
         <v>4</v>
       </c>
       <c r="C227" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D227" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -3670,10 +3667,10 @@
         <v>7</v>
       </c>
       <c r="C228" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D228" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -3684,10 +3681,10 @@
         <v>10</v>
       </c>
       <c r="C229" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D229" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -3695,13 +3692,13 @@
         <v>46</v>
       </c>
       <c r="B230" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C230" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D230" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -3709,13 +3706,13 @@
         <v>46</v>
       </c>
       <c r="B231" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C231" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D231" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -3729,7 +3726,7 @@
         <v>11</v>
       </c>
       <c r="D232" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -3740,10 +3737,10 @@
         <v>7</v>
       </c>
       <c r="C233" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D233" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -3754,10 +3751,10 @@
         <v>10</v>
       </c>
       <c r="C234" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D234" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -3765,10 +3762,10 @@
         <v>47</v>
       </c>
       <c r="B235" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C235" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D235" t="s">
         <v>6</v>
@@ -3779,13 +3776,13 @@
         <v>47</v>
       </c>
       <c r="B236" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C236" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D236" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -3796,10 +3793,10 @@
         <v>4</v>
       </c>
       <c r="C237" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D237" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
@@ -3810,10 +3807,10 @@
         <v>7</v>
       </c>
       <c r="C238" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D238" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -3824,10 +3821,10 @@
         <v>10</v>
       </c>
       <c r="C239" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D239" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -3835,13 +3832,13 @@
         <v>48</v>
       </c>
       <c r="B240" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C240" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D240" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -3849,13 +3846,13 @@
         <v>48</v>
       </c>
       <c r="B241" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C241" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D241" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -3866,7 +3863,7 @@
         <v>4</v>
       </c>
       <c r="C242" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D242" t="s">
         <v>6</v>
@@ -3880,10 +3877,10 @@
         <v>7</v>
       </c>
       <c r="C243" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D243" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -3894,10 +3891,10 @@
         <v>10</v>
       </c>
       <c r="C244" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D244" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -3905,10 +3902,10 @@
         <v>49</v>
       </c>
       <c r="B245" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C245" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D245" t="s">
         <v>9</v>
@@ -3919,13 +3916,13 @@
         <v>49</v>
       </c>
       <c r="B246" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C246" t="s">
         <v>8</v>
       </c>
       <c r="D246" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -3950,7 +3947,7 @@
         <v>7</v>
       </c>
       <c r="C248" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D248" t="s">
         <v>6</v>
@@ -3964,10 +3961,10 @@
         <v>10</v>
       </c>
       <c r="C249" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D249" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -3975,13 +3972,13 @@
         <v>50</v>
       </c>
       <c r="B250" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C250" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D250" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -3989,13 +3986,13 @@
         <v>50</v>
       </c>
       <c r="B251" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C251" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D251" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -4006,10 +4003,10 @@
         <v>4</v>
       </c>
       <c r="C252" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D252" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
@@ -4020,7 +4017,7 @@
         <v>7</v>
       </c>
       <c r="C253" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D253" t="s">
         <v>6</v>
@@ -4034,10 +4031,10 @@
         <v>10</v>
       </c>
       <c r="C254" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D254" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -4045,13 +4042,13 @@
         <v>51</v>
       </c>
       <c r="B255" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C255" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D255" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -4059,13 +4056,13 @@
         <v>51</v>
       </c>
       <c r="B256" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C256" t="s">
         <v>8</v>
       </c>
       <c r="D256" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -4076,10 +4073,10 @@
         <v>4</v>
       </c>
       <c r="C257" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D257" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -4090,10 +4087,10 @@
         <v>7</v>
       </c>
       <c r="C258" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D258" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -4104,10 +4101,10 @@
         <v>10</v>
       </c>
       <c r="C259" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D259" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -4115,13 +4112,13 @@
         <v>52</v>
       </c>
       <c r="B260" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C260" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D260" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -4129,13 +4126,13 @@
         <v>52</v>
       </c>
       <c r="B261" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C261" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D261" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>